<commit_message>
Updated weekly rate data
</commit_message>
<xml_diff>
--- a/case_data.xlsx
+++ b/case_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timothywiemken/Dropbox/Work/pfizer/covid epi/case by age 2021/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timothywiemken/Dropbox/Work/pfizer/covid epi/pediatric fda letter/GitHub Code/covid-agegroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635FC002-5664-A544-98BD-DF7412694815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C805A68-D46D-4243-AF00-65922517F5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="500" windowWidth="13840" windowHeight="17500" xr2:uid="{CC2C058F-5A66-1E4E-8340-2D9DC2FB7952}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="12280" windowHeight="13900" xr2:uid="{CC2C058F-5A66-1E4E-8340-2D9DC2FB7952}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14FFA509-206F-304C-A5FE-F366C177BBC6}">
-  <dimension ref="A1:K78"/>
+  <dimension ref="A1:K79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="L79" sqref="L79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3157,6 +3157,41 @@
         <v>42.8</v>
       </c>
     </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>44436</v>
+      </c>
+      <c r="B79">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="C79">
+        <v>120.8</v>
+      </c>
+      <c r="D79">
+        <v>141.6</v>
+      </c>
+      <c r="E79">
+        <v>148.1</v>
+      </c>
+      <c r="F79">
+        <v>136.80000000000001</v>
+      </c>
+      <c r="G79">
+        <v>138.30000000000001</v>
+      </c>
+      <c r="H79">
+        <v>119.7</v>
+      </c>
+      <c r="I79">
+        <v>90</v>
+      </c>
+      <c r="J79">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="K79">
+        <v>60.6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated data for cases from CDC
https://covid.cdc.gov/covid-data-tracker/#demographicsovertime
</commit_message>
<xml_diff>
--- a/case_data.xlsx
+++ b/case_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timothywiemken/Dropbox/Work/pfizer/covid epi/pediatric fda letter/GitHub Code/covid-agegroups/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timwiemken/Library/Mobile Documents/com~apple~CloudDocs/Work/Pfizer/FDA/COVID pediatric fda letter/GitHub Code/covid-agegroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C805A68-D46D-4243-AF00-65922517F5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F96D3B-E541-6F4C-82D2-4F825ACD3499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="12280" windowHeight="13900" xr2:uid="{CC2C058F-5A66-1E4E-8340-2D9DC2FB7952}"/>
+    <workbookView xWindow="1200" yWindow="500" windowWidth="27600" windowHeight="17500" xr2:uid="{CC2C058F-5A66-1E4E-8340-2D9DC2FB7952}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14FFA509-206F-304C-A5FE-F366C177BBC6}">
-  <dimension ref="A1:K79"/>
+  <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L79" sqref="L79"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="F95" sqref="F95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3192,6 +3192,111 @@
         <v>60.6</v>
       </c>
     </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>44443</v>
+      </c>
+      <c r="B80">
+        <v>121.1</v>
+      </c>
+      <c r="C80">
+        <v>228.1</v>
+      </c>
+      <c r="D80">
+        <v>264.5</v>
+      </c>
+      <c r="E80">
+        <v>274.2</v>
+      </c>
+      <c r="F80">
+        <v>218.6</v>
+      </c>
+      <c r="G80">
+        <v>223.1</v>
+      </c>
+      <c r="H80">
+        <v>192</v>
+      </c>
+      <c r="I80">
+        <v>142.9</v>
+      </c>
+      <c r="J80">
+        <v>109.3</v>
+      </c>
+      <c r="K80">
+        <v>99.1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>44450</v>
+      </c>
+      <c r="B81">
+        <v>89.6</v>
+      </c>
+      <c r="C81">
+        <v>165.7</v>
+      </c>
+      <c r="D81">
+        <v>192.3</v>
+      </c>
+      <c r="E81">
+        <v>198.8</v>
+      </c>
+      <c r="F81">
+        <v>162.1</v>
+      </c>
+      <c r="G81">
+        <v>166.1</v>
+      </c>
+      <c r="H81">
+        <v>145.80000000000001</v>
+      </c>
+      <c r="I81">
+        <v>109.1</v>
+      </c>
+      <c r="J81">
+        <v>82.8</v>
+      </c>
+      <c r="K81">
+        <v>75.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>44457</v>
+      </c>
+      <c r="B82">
+        <v>7.7</v>
+      </c>
+      <c r="C82">
+        <v>13.5</v>
+      </c>
+      <c r="D82">
+        <v>17.7</v>
+      </c>
+      <c r="E82">
+        <v>18.2</v>
+      </c>
+      <c r="F82">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="G82">
+        <v>15.8</v>
+      </c>
+      <c r="H82">
+        <v>13.8</v>
+      </c>
+      <c r="I82">
+        <v>10.4</v>
+      </c>
+      <c r="J82">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="K82">
+        <v>7.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated data from CDC
</commit_message>
<xml_diff>
--- a/case_data.xlsx
+++ b/case_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timothywiemken/Dropbox/Work/pfizer/covid epi/pediatric fda letter/GitHub Code/covid-agegroups/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timwiemken/Library/Mobile Documents/com~apple~CloudDocs/Work/Pfizer/COVID pediatric case count/count github/covid-agegroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C805A68-D46D-4243-AF00-65922517F5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89C7AC1-4497-AF40-AAEA-04C526C8C1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="12280" windowHeight="13900" xr2:uid="{CC2C058F-5A66-1E4E-8340-2D9DC2FB7952}"/>
+    <workbookView xWindow="1200" yWindow="500" windowWidth="27600" windowHeight="17500" xr2:uid="{CC2C058F-5A66-1E4E-8340-2D9DC2FB7952}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14FFA509-206F-304C-A5FE-F366C177BBC6}">
-  <dimension ref="A1:K79"/>
+  <dimension ref="A1:K81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L79" sqref="L79"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3192,6 +3192,76 @@
         <v>60.6</v>
       </c>
     </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>44443</v>
+      </c>
+      <c r="B80">
+        <v>121.1</v>
+      </c>
+      <c r="C80">
+        <v>228.1</v>
+      </c>
+      <c r="D80">
+        <v>264.5</v>
+      </c>
+      <c r="E80">
+        <v>274.2</v>
+      </c>
+      <c r="F80">
+        <v>218.6</v>
+      </c>
+      <c r="G80">
+        <v>223.1</v>
+      </c>
+      <c r="H80">
+        <v>192</v>
+      </c>
+      <c r="I80">
+        <v>142.9</v>
+      </c>
+      <c r="J80">
+        <v>109.3</v>
+      </c>
+      <c r="K80">
+        <v>99.1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>44450</v>
+      </c>
+      <c r="B81">
+        <v>89.6</v>
+      </c>
+      <c r="C81">
+        <v>165.7</v>
+      </c>
+      <c r="D81">
+        <v>192.3</v>
+      </c>
+      <c r="E81">
+        <v>198.8</v>
+      </c>
+      <c r="F81">
+        <v>162.1</v>
+      </c>
+      <c r="G81">
+        <v>166.1</v>
+      </c>
+      <c r="H81">
+        <v>145.80000000000001</v>
+      </c>
+      <c r="I81">
+        <v>109.1</v>
+      </c>
+      <c r="J81">
+        <v>82.8</v>
+      </c>
+      <c r="K81">
+        <v>75.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Rates from CDC Through 9/18
</commit_message>
<xml_diff>
--- a/case_data.xlsx
+++ b/case_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timwiemken/Library/Mobile Documents/com~apple~CloudDocs/Work/Pfizer/COVID pediatric case count/count github/covid-agegroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4CF3BD-5FCB-F040-96DC-C9D26C26F3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A64667D-6D84-8842-859F-077D40D08BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="500" windowWidth="27600" windowHeight="17500" xr2:uid="{CC2C058F-5A66-1E4E-8340-2D9DC2FB7952}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -419,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14FFA509-206F-304C-A5FE-F366C177BBC6}">
-  <dimension ref="A1:K81"/>
+  <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="M76" sqref="M76"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,19 +518,19 @@
         <v>8.4</v>
       </c>
       <c r="G3">
-        <v>12</v>
+        <v>12.1</v>
       </c>
       <c r="H3">
         <v>14.5</v>
       </c>
       <c r="I3">
-        <v>15.1</v>
+        <v>15.2</v>
       </c>
       <c r="J3">
-        <v>13.2</v>
+        <v>13.3</v>
       </c>
       <c r="K3">
-        <v>11.7</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -552,19 +553,19 @@
         <v>30</v>
       </c>
       <c r="G4">
-        <v>42</v>
+        <v>42.2</v>
       </c>
       <c r="H4">
-        <v>47.8</v>
+        <v>47.9</v>
       </c>
       <c r="I4">
-        <v>48.8</v>
+        <v>49.1</v>
       </c>
       <c r="J4">
-        <v>39.5</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="K4">
-        <v>35.9</v>
+        <v>36.200000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -584,22 +585,22 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="F5">
-        <v>36.4</v>
+        <v>36.6</v>
       </c>
       <c r="G5">
-        <v>56.6</v>
+        <v>57</v>
       </c>
       <c r="H5">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="I5">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="J5">
+        <v>54.2</v>
+      </c>
+      <c r="K5">
         <v>65.2</v>
-      </c>
-      <c r="I5">
-        <v>68.5</v>
-      </c>
-      <c r="J5">
-        <v>53.8</v>
-      </c>
-      <c r="K5">
-        <v>64.5</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -607,34 +608,34 @@
         <v>43925</v>
       </c>
       <c r="B6">
-        <v>4.3</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C6">
         <v>3.4</v>
       </c>
       <c r="D6">
-        <v>5.9</v>
+        <v>6</v>
       </c>
       <c r="E6">
-        <v>10.8</v>
+        <v>10.9</v>
       </c>
       <c r="F6">
-        <v>43.1</v>
+        <v>43.4</v>
       </c>
       <c r="G6">
-        <v>65</v>
+        <v>65.599999999999994</v>
       </c>
       <c r="H6">
-        <v>76.8</v>
+        <v>77.400000000000006</v>
       </c>
       <c r="I6">
-        <v>82.5</v>
+        <v>83.4</v>
       </c>
       <c r="J6">
-        <v>65</v>
+        <v>66.2</v>
       </c>
       <c r="K6">
-        <v>94.7</v>
+        <v>96.7</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -642,34 +643,34 @@
         <v>43932</v>
       </c>
       <c r="B7">
-        <v>5.6</v>
+        <v>5.7</v>
       </c>
       <c r="C7">
         <v>4.2</v>
       </c>
       <c r="D7">
-        <v>7.1</v>
+        <v>7.2</v>
       </c>
       <c r="E7">
-        <v>13.4</v>
+        <v>13.5</v>
       </c>
       <c r="F7">
-        <v>45.6</v>
+        <v>45.9</v>
       </c>
       <c r="G7">
-        <v>64</v>
+        <v>64.5</v>
       </c>
       <c r="H7">
-        <v>76.599999999999994</v>
+        <v>77.2</v>
       </c>
       <c r="I7">
-        <v>81.400000000000006</v>
+        <v>82.2</v>
       </c>
       <c r="J7">
-        <v>67</v>
+        <v>67.900000000000006</v>
       </c>
       <c r="K7">
-        <v>121.8</v>
+        <v>124.1</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -680,31 +681,31 @@
         <v>5.6</v>
       </c>
       <c r="C8">
-        <v>4.9000000000000004</v>
+        <v>5</v>
       </c>
       <c r="D8">
-        <v>8.6</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="E8">
-        <v>14.9</v>
+        <v>15</v>
       </c>
       <c r="F8">
-        <v>45.6</v>
+        <v>46</v>
       </c>
       <c r="G8">
-        <v>60.3</v>
+        <v>60.9</v>
       </c>
       <c r="H8">
-        <v>68.5</v>
+        <v>69.099999999999994</v>
       </c>
       <c r="I8">
-        <v>70.5</v>
+        <v>71.3</v>
       </c>
       <c r="J8">
-        <v>57.9</v>
+        <v>58.6</v>
       </c>
       <c r="K8">
-        <v>118.6</v>
+        <v>120.8</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -718,28 +719,28 @@
         <v>6.8</v>
       </c>
       <c r="D9">
-        <v>11.9</v>
+        <v>12.1</v>
       </c>
       <c r="E9">
-        <v>19.899999999999999</v>
+        <v>20</v>
       </c>
       <c r="F9">
-        <v>53.7</v>
+        <v>54.2</v>
       </c>
       <c r="G9">
-        <v>66.900000000000006</v>
+        <v>67.7</v>
       </c>
       <c r="H9">
-        <v>75.099999999999994</v>
+        <v>75.7</v>
       </c>
       <c r="I9">
-        <v>71.8</v>
+        <v>72.400000000000006</v>
       </c>
       <c r="J9">
-        <v>56.3</v>
+        <v>56.7</v>
       </c>
       <c r="K9">
-        <v>117.8</v>
+        <v>118.2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -747,34 +748,34 @@
         <v>43953</v>
       </c>
       <c r="B10">
-        <v>9.1</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="C10">
-        <v>8.6</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="D10">
-        <v>14.8</v>
+        <v>14.9</v>
       </c>
       <c r="E10">
-        <v>25.1</v>
+        <v>25.3</v>
       </c>
       <c r="F10">
-        <v>61.2</v>
+        <v>61.7</v>
       </c>
       <c r="G10">
-        <v>70.900000000000006</v>
+        <v>71.599999999999994</v>
       </c>
       <c r="H10">
-        <v>77.400000000000006</v>
+        <v>77.900000000000006</v>
       </c>
       <c r="I10">
-        <v>69.8</v>
+        <v>70</v>
       </c>
       <c r="J10">
-        <v>52.4</v>
+        <v>52.3</v>
       </c>
       <c r="K10">
-        <v>104.7</v>
+        <v>104.1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -782,34 +783,34 @@
         <v>43960</v>
       </c>
       <c r="B11">
-        <v>9.6999999999999993</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C11">
-        <v>10</v>
+        <v>10.1</v>
       </c>
       <c r="D11">
-        <v>16.2</v>
+        <v>16.3</v>
       </c>
       <c r="E11">
-        <v>26.3</v>
+        <v>26.5</v>
       </c>
       <c r="F11">
-        <v>54.7</v>
+        <v>55.2</v>
       </c>
       <c r="G11">
-        <v>62.1</v>
+        <v>62.7</v>
       </c>
       <c r="H11">
-        <v>64.2</v>
+        <v>64.8</v>
       </c>
       <c r="I11">
-        <v>58.9</v>
+        <v>59.3</v>
       </c>
       <c r="J11">
-        <v>44.6</v>
+        <v>44.8</v>
       </c>
       <c r="K11">
-        <v>83</v>
+        <v>83.2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -817,34 +818,34 @@
         <v>43967</v>
       </c>
       <c r="B12">
-        <v>12.1</v>
+        <v>12.2</v>
       </c>
       <c r="C12">
-        <v>11.9</v>
+        <v>12</v>
       </c>
       <c r="D12">
         <v>19</v>
       </c>
       <c r="E12">
-        <v>29.9</v>
+        <v>30.1</v>
       </c>
       <c r="F12">
-        <v>57.9</v>
+        <v>58.2</v>
       </c>
       <c r="G12">
-        <v>63.1</v>
+        <v>63.5</v>
       </c>
       <c r="H12">
-        <v>65.400000000000006</v>
+        <v>65.7</v>
       </c>
       <c r="I12">
-        <v>58.5</v>
+        <v>58.9</v>
       </c>
       <c r="J12">
-        <v>43.4</v>
+        <v>43.5</v>
       </c>
       <c r="K12">
-        <v>79.400000000000006</v>
+        <v>79.8</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -864,22 +865,22 @@
         <v>30.4</v>
       </c>
       <c r="F13">
-        <v>59.1</v>
+        <v>59.4</v>
       </c>
       <c r="G13">
-        <v>62.3</v>
+        <v>62.6</v>
       </c>
       <c r="H13">
-        <v>63.9</v>
+        <v>64.099999999999994</v>
       </c>
       <c r="I13">
-        <v>54.4</v>
+        <v>54.5</v>
       </c>
       <c r="J13">
-        <v>39.4</v>
+        <v>39.5</v>
       </c>
       <c r="K13">
-        <v>65</v>
+        <v>65.400000000000006</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -890,31 +891,31 @@
         <v>12.7</v>
       </c>
       <c r="C14">
-        <v>13</v>
+        <v>13.1</v>
       </c>
       <c r="D14">
-        <v>20.100000000000001</v>
+        <v>20.2</v>
       </c>
       <c r="E14">
-        <v>30.3</v>
+        <v>30.5</v>
       </c>
       <c r="F14">
+        <v>58.8</v>
+      </c>
+      <c r="G14">
+        <v>60.6</v>
+      </c>
+      <c r="H14">
+        <v>59.4</v>
+      </c>
+      <c r="I14">
+        <v>50.1</v>
+      </c>
+      <c r="J14">
+        <v>34.6</v>
+      </c>
+      <c r="K14">
         <v>58.6</v>
-      </c>
-      <c r="G14">
-        <v>60.3</v>
-      </c>
-      <c r="H14">
-        <v>59.2</v>
-      </c>
-      <c r="I14">
-        <v>49.9</v>
-      </c>
-      <c r="J14">
-        <v>34.5</v>
-      </c>
-      <c r="K14">
-        <v>58.4</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -922,34 +923,34 @@
         <v>43988</v>
       </c>
       <c r="B15">
-        <v>13.8</v>
+        <v>13.9</v>
       </c>
       <c r="C15">
         <v>14.1</v>
       </c>
       <c r="D15">
-        <v>20.9</v>
+        <v>21</v>
       </c>
       <c r="E15">
         <v>33.299999999999997</v>
       </c>
       <c r="F15">
-        <v>60.4</v>
+        <v>60.5</v>
       </c>
       <c r="G15">
         <v>56.6</v>
       </c>
       <c r="H15">
-        <v>56.7</v>
+        <v>56.8</v>
       </c>
       <c r="I15">
-        <v>46.1</v>
+        <v>46.2</v>
       </c>
       <c r="J15">
-        <v>32.4</v>
+        <v>32.5</v>
       </c>
       <c r="K15">
-        <v>49.2</v>
+        <v>49.3</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -966,25 +967,25 @@
         <v>24.1</v>
       </c>
       <c r="E16">
-        <v>37.4</v>
+        <v>37.5</v>
       </c>
       <c r="F16">
-        <v>74.3</v>
+        <v>74.5</v>
       </c>
       <c r="G16">
-        <v>63.3</v>
+        <v>63.4</v>
       </c>
       <c r="H16">
-        <v>61.4</v>
+        <v>61.5</v>
       </c>
       <c r="I16">
-        <v>48.5</v>
+        <v>48.6</v>
       </c>
       <c r="J16">
-        <v>34.5</v>
+        <v>34.6</v>
       </c>
       <c r="K16">
-        <v>46.5</v>
+        <v>46.6</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1004,7 +1005,7 @@
         <v>50.7</v>
       </c>
       <c r="F17">
-        <v>110.4</v>
+        <v>110.5</v>
       </c>
       <c r="G17">
         <v>88.1</v>
@@ -1013,13 +1014,13 @@
         <v>82.1</v>
       </c>
       <c r="I17">
-        <v>63.1</v>
+        <v>63</v>
       </c>
       <c r="J17">
-        <v>42.5</v>
+        <v>42.4</v>
       </c>
       <c r="K17">
-        <v>51.4</v>
+        <v>51.3</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -1033,28 +1034,28 @@
         <v>25.9</v>
       </c>
       <c r="D18">
-        <v>37.200000000000003</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="E18">
-        <v>67.2</v>
+        <v>67.400000000000006</v>
       </c>
       <c r="F18">
-        <v>148.4</v>
+        <v>148.80000000000001</v>
       </c>
       <c r="G18">
-        <v>113.7</v>
+        <v>114</v>
       </c>
       <c r="H18">
-        <v>100.4</v>
+        <v>100.7</v>
       </c>
       <c r="I18">
-        <v>79.5</v>
+        <v>79.7</v>
       </c>
       <c r="J18">
-        <v>52.6</v>
+        <v>52.7</v>
       </c>
       <c r="K18">
-        <v>66.3</v>
+        <v>66.400000000000006</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -1062,34 +1063,34 @@
         <v>44016</v>
       </c>
       <c r="B19">
-        <v>27.9</v>
+        <v>28</v>
       </c>
       <c r="C19">
-        <v>28</v>
+        <v>28.1</v>
       </c>
       <c r="D19">
-        <v>44.6</v>
+        <v>44.8</v>
       </c>
       <c r="E19">
-        <v>79.8</v>
+        <v>80</v>
       </c>
       <c r="F19">
-        <v>159.5</v>
+        <v>160.1</v>
       </c>
       <c r="G19">
-        <v>122.4</v>
+        <v>122.7</v>
       </c>
       <c r="H19">
-        <v>112.1</v>
+        <v>112.3</v>
       </c>
       <c r="I19">
-        <v>86.6</v>
+        <v>86.9</v>
       </c>
       <c r="J19">
-        <v>56.6</v>
+        <v>56.8</v>
       </c>
       <c r="K19">
-        <v>61.4</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -1097,34 +1098,34 @@
         <v>44023</v>
       </c>
       <c r="B20">
-        <v>32.299999999999997</v>
+        <v>32.4</v>
       </c>
       <c r="C20">
-        <v>34</v>
+        <v>34.1</v>
       </c>
       <c r="D20">
         <v>53.9</v>
       </c>
       <c r="E20">
-        <v>98.7</v>
+        <v>99</v>
       </c>
       <c r="F20">
-        <v>174.1</v>
+        <v>174.6</v>
       </c>
       <c r="G20">
-        <v>136.80000000000001</v>
+        <v>137.1</v>
       </c>
       <c r="H20">
-        <v>127.7</v>
+        <v>128</v>
       </c>
       <c r="I20">
-        <v>99.3</v>
+        <v>99.6</v>
       </c>
       <c r="J20">
-        <v>66.2</v>
+        <v>66.400000000000006</v>
       </c>
       <c r="K20">
-        <v>71.400000000000006</v>
+        <v>71.5</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -1132,31 +1133,31 @@
         <v>44030</v>
       </c>
       <c r="B21">
-        <v>33.6</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="C21">
-        <v>35.799999999999997</v>
+        <v>35.9</v>
       </c>
       <c r="D21">
-        <v>58.1</v>
+        <v>58.3</v>
       </c>
       <c r="E21">
-        <v>101</v>
+        <v>101.2</v>
       </c>
       <c r="F21">
-        <v>163.1</v>
+        <v>163.6</v>
       </c>
       <c r="G21">
-        <v>133.69999999999999</v>
+        <v>134.1</v>
       </c>
       <c r="H21">
-        <v>127.1</v>
+        <v>127.3</v>
       </c>
       <c r="I21">
-        <v>101.8</v>
+        <v>102</v>
       </c>
       <c r="J21">
-        <v>69.599999999999994</v>
+        <v>69.8</v>
       </c>
       <c r="K21">
         <v>77.599999999999994</v>
@@ -1167,34 +1168,34 @@
         <v>44037</v>
       </c>
       <c r="B22">
-        <v>32.799999999999997</v>
+        <v>32.9</v>
       </c>
       <c r="C22">
-        <v>35.1</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="D22">
-        <v>54.7</v>
+        <v>54.9</v>
       </c>
       <c r="E22">
-        <v>93</v>
+        <v>93.5</v>
       </c>
       <c r="F22">
-        <v>143.5</v>
+        <v>144.1</v>
       </c>
       <c r="G22">
-        <v>120.6</v>
+        <v>121.1</v>
       </c>
       <c r="H22">
-        <v>118.2</v>
+        <v>118.7</v>
       </c>
       <c r="I22">
-        <v>94.8</v>
+        <v>95.2</v>
       </c>
       <c r="J22">
-        <v>67.5</v>
+        <v>67.7</v>
       </c>
       <c r="K22">
-        <v>75.599999999999994</v>
+        <v>75.900000000000006</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -1205,31 +1206,31 @@
         <v>30.3</v>
       </c>
       <c r="C23">
-        <v>32.6</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="D23">
-        <v>52.3</v>
+        <v>52.4</v>
       </c>
       <c r="E23">
+        <v>88.7</v>
+      </c>
+      <c r="F23">
+        <v>129.30000000000001</v>
+      </c>
+      <c r="G23">
+        <v>108.2</v>
+      </c>
+      <c r="H23">
+        <v>108</v>
+      </c>
+      <c r="I23">
         <v>88.3</v>
       </c>
-      <c r="F23">
-        <v>128.9</v>
-      </c>
-      <c r="G23">
-        <v>107.9</v>
-      </c>
-      <c r="H23">
-        <v>107.7</v>
-      </c>
-      <c r="I23">
-        <v>88.1</v>
-      </c>
       <c r="J23">
-        <v>63.9</v>
+        <v>64</v>
       </c>
       <c r="K23">
-        <v>73.5</v>
+        <v>73.599999999999994</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -1243,28 +1244,28 @@
         <v>29.5</v>
       </c>
       <c r="D24">
-        <v>46.6</v>
+        <v>46.7</v>
       </c>
       <c r="E24">
-        <v>79.3</v>
+        <v>79.599999999999994</v>
       </c>
       <c r="F24">
-        <v>112.8</v>
+        <v>113.1</v>
       </c>
       <c r="G24">
-        <v>92.2</v>
+        <v>92.4</v>
       </c>
       <c r="H24">
-        <v>91.7</v>
+        <v>92</v>
       </c>
       <c r="I24">
-        <v>76.3</v>
+        <v>76.5</v>
       </c>
       <c r="J24">
-        <v>54.9</v>
+        <v>55</v>
       </c>
       <c r="K24">
-        <v>65.099999999999994</v>
+        <v>65.3</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -1272,34 +1273,34 @@
         <v>44058</v>
       </c>
       <c r="B25">
-        <v>26.1</v>
+        <v>26</v>
       </c>
       <c r="C25">
-        <v>29.3</v>
+        <v>29.2</v>
       </c>
       <c r="D25">
-        <v>44.6</v>
+        <v>44.2</v>
       </c>
       <c r="E25">
-        <v>76.099999999999994</v>
+        <v>75.8</v>
       </c>
       <c r="F25">
-        <v>111.8</v>
+        <v>111.5</v>
       </c>
       <c r="G25">
-        <v>89.2</v>
+        <v>88.8</v>
       </c>
       <c r="H25">
-        <v>88.3</v>
+        <v>88</v>
       </c>
       <c r="I25">
-        <v>73.7</v>
+        <v>73.5</v>
       </c>
       <c r="J25">
-        <v>54.1</v>
+        <v>54</v>
       </c>
       <c r="K25">
-        <v>63</v>
+        <v>62.8</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -1307,34 +1308,34 @@
         <v>44065</v>
       </c>
       <c r="B26">
-        <v>26.7</v>
+        <v>26.8</v>
       </c>
       <c r="C26">
-        <v>29.7</v>
+        <v>29.8</v>
       </c>
       <c r="D26">
-        <v>44.6</v>
+        <v>44.8</v>
       </c>
       <c r="E26">
-        <v>75.5</v>
+        <v>76</v>
       </c>
       <c r="F26">
-        <v>131.9</v>
+        <v>132.6</v>
       </c>
       <c r="G26">
-        <v>96.3</v>
+        <v>96.9</v>
       </c>
       <c r="H26">
-        <v>95.7</v>
+        <v>96.2</v>
       </c>
       <c r="I26">
-        <v>79.8</v>
+        <v>80.3</v>
       </c>
       <c r="J26">
-        <v>58.6</v>
+        <v>59</v>
       </c>
       <c r="K26">
-        <v>68.400000000000006</v>
+        <v>68.8</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -1342,34 +1343,34 @@
         <v>44072</v>
       </c>
       <c r="B27">
-        <v>22.2</v>
+        <v>22.4</v>
       </c>
       <c r="C27">
-        <v>25.7</v>
+        <v>25.9</v>
       </c>
       <c r="D27">
-        <v>39.1</v>
+        <v>39.4</v>
       </c>
       <c r="E27">
-        <v>66.099999999999994</v>
+        <v>66.7</v>
       </c>
       <c r="F27">
-        <v>136.4</v>
+        <v>137.4</v>
       </c>
       <c r="G27">
-        <v>76.5</v>
+        <v>77</v>
       </c>
       <c r="H27">
-        <v>75.900000000000006</v>
+        <v>76.3</v>
       </c>
       <c r="I27">
-        <v>64</v>
+        <v>64.400000000000006</v>
       </c>
       <c r="J27">
-        <v>46.8</v>
+        <v>47.1</v>
       </c>
       <c r="K27">
-        <v>55.4</v>
+        <v>55.7</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -1377,34 +1378,34 @@
         <v>44079</v>
       </c>
       <c r="B28">
-        <v>18.600000000000001</v>
+        <v>18.8</v>
       </c>
       <c r="C28">
-        <v>21</v>
+        <v>21.3</v>
       </c>
       <c r="D28">
-        <v>36.299999999999997</v>
+        <v>36.799999999999997</v>
       </c>
       <c r="E28">
-        <v>63.5</v>
+        <v>64.099999999999994</v>
       </c>
       <c r="F28">
-        <v>135</v>
+        <v>136.6</v>
       </c>
       <c r="G28">
-        <v>63.1</v>
+        <v>63.9</v>
       </c>
       <c r="H28">
-        <v>63.9</v>
+        <v>64.7</v>
       </c>
       <c r="I28">
-        <v>55</v>
+        <v>55.7</v>
       </c>
       <c r="J28">
-        <v>41.7</v>
+        <v>42.2</v>
       </c>
       <c r="K28">
-        <v>51.6</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -1412,34 +1413,34 @@
         <v>44086</v>
       </c>
       <c r="B29">
-        <v>17.2</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="C29">
-        <v>21.7</v>
+        <v>22</v>
       </c>
       <c r="D29">
-        <v>37.1</v>
+        <v>37.6</v>
       </c>
       <c r="E29">
+        <v>65.7</v>
+      </c>
+      <c r="F29">
+        <v>122.6</v>
+      </c>
+      <c r="G29">
+        <v>64.5</v>
+      </c>
+      <c r="H29">
         <v>64.7</v>
       </c>
-      <c r="F29">
-        <v>121.2</v>
-      </c>
-      <c r="G29">
-        <v>63.6</v>
-      </c>
-      <c r="H29">
-        <v>63.9</v>
-      </c>
       <c r="I29">
-        <v>56.2</v>
+        <v>57</v>
       </c>
       <c r="J29">
-        <v>42.9</v>
+        <v>43.3</v>
       </c>
       <c r="K29">
-        <v>49.9</v>
+        <v>50.3</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -1447,34 +1448,34 @@
         <v>44093</v>
       </c>
       <c r="B30">
-        <v>22.6</v>
+        <v>23.1</v>
       </c>
       <c r="C30">
-        <v>28.4</v>
+        <v>28.9</v>
       </c>
       <c r="D30">
-        <v>48.2</v>
+        <v>48.9</v>
       </c>
       <c r="E30">
-        <v>79.2</v>
+        <v>80.8</v>
       </c>
       <c r="F30">
-        <v>134.19999999999999</v>
+        <v>133.69999999999999</v>
       </c>
       <c r="G30">
-        <v>82.9</v>
+        <v>84.1</v>
       </c>
       <c r="H30">
-        <v>82.4</v>
+        <v>83.5</v>
       </c>
       <c r="I30">
-        <v>71.099999999999994</v>
+        <v>72</v>
       </c>
       <c r="J30">
-        <v>53.8</v>
+        <v>54.5</v>
       </c>
       <c r="K30">
-        <v>62.8</v>
+        <v>63.4</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -1482,34 +1483,34 @@
         <v>44100</v>
       </c>
       <c r="B31">
-        <v>25.1</v>
+        <v>25.6</v>
       </c>
       <c r="C31">
-        <v>30.7</v>
+        <v>31.2</v>
       </c>
       <c r="D31">
-        <v>52.6</v>
+        <v>53.8</v>
       </c>
       <c r="E31">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F31">
-        <v>132.30000000000001</v>
+        <v>130.9</v>
       </c>
       <c r="G31">
-        <v>91.9</v>
+        <v>93.6</v>
       </c>
       <c r="H31">
-        <v>91.8</v>
+        <v>93.6</v>
       </c>
       <c r="I31">
-        <v>80.099999999999994</v>
+        <v>81.3</v>
       </c>
       <c r="J31">
-        <v>62.3</v>
+        <v>63.1</v>
       </c>
       <c r="K31">
-        <v>70.2</v>
+        <v>70.900000000000006</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -1517,34 +1518,34 @@
         <v>44107</v>
       </c>
       <c r="B32">
-        <v>26.6</v>
+        <v>27.2</v>
       </c>
       <c r="C32">
-        <v>34.1</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="D32">
-        <v>56.5</v>
+        <v>57.6</v>
       </c>
       <c r="E32">
-        <v>83.7</v>
+        <v>85.2</v>
       </c>
       <c r="F32">
-        <v>126.8</v>
+        <v>129.19999999999999</v>
       </c>
       <c r="G32">
-        <v>98.5</v>
+        <v>100.4</v>
       </c>
       <c r="H32">
-        <v>98.1</v>
+        <v>99.8</v>
       </c>
       <c r="I32">
-        <v>87.1</v>
+        <v>88.7</v>
       </c>
       <c r="J32">
-        <v>71.3</v>
+        <v>72.400000000000006</v>
       </c>
       <c r="K32">
-        <v>78.900000000000006</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -1552,34 +1553,34 @@
         <v>44114</v>
       </c>
       <c r="B33">
-        <v>28.5</v>
+        <v>29.7</v>
       </c>
       <c r="C33">
-        <v>37.700000000000003</v>
+        <v>39</v>
       </c>
       <c r="D33">
-        <v>63.8</v>
+        <v>65.8</v>
       </c>
       <c r="E33">
-        <v>93.9</v>
+        <v>97</v>
       </c>
       <c r="F33">
-        <v>143.1</v>
+        <v>135.80000000000001</v>
       </c>
       <c r="G33">
-        <v>106.1</v>
+        <v>109.5</v>
       </c>
       <c r="H33">
-        <v>107.1</v>
+        <v>110.5</v>
       </c>
       <c r="I33">
-        <v>96.7</v>
+        <v>99.2</v>
       </c>
       <c r="J33">
-        <v>77.599999999999994</v>
+        <v>79.599999999999994</v>
       </c>
       <c r="K33">
-        <v>85.9</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -1587,34 +1588,34 @@
         <v>44121</v>
       </c>
       <c r="B34">
-        <v>35.1</v>
+        <v>35.9</v>
       </c>
       <c r="C34">
-        <v>45.2</v>
+        <v>46.1</v>
       </c>
       <c r="D34">
-        <v>76.2</v>
+        <v>78.099999999999994</v>
       </c>
       <c r="E34">
-        <v>110.6</v>
+        <v>113.2</v>
       </c>
       <c r="F34">
-        <v>164.4</v>
+        <v>159.69999999999999</v>
       </c>
       <c r="G34">
-        <v>133.19999999999999</v>
+        <v>136.5</v>
       </c>
       <c r="H34">
-        <v>133.9</v>
+        <v>136.9</v>
       </c>
       <c r="I34">
-        <v>120.5</v>
+        <v>122.8</v>
       </c>
       <c r="J34">
-        <v>93.2</v>
+        <v>95</v>
       </c>
       <c r="K34">
-        <v>104.8</v>
+        <v>106.9</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
@@ -1622,34 +1623,34 @@
         <v>44128</v>
       </c>
       <c r="B35">
-        <v>43.3</v>
+        <v>44.3</v>
       </c>
       <c r="C35">
-        <v>58.3</v>
+        <v>59.6</v>
       </c>
       <c r="D35">
-        <v>97</v>
+        <v>99.4</v>
       </c>
       <c r="E35">
-        <v>140.9</v>
+        <v>144.5</v>
       </c>
       <c r="F35">
-        <v>211.7</v>
+        <v>205</v>
       </c>
       <c r="G35">
-        <v>173.4</v>
+        <v>177</v>
       </c>
       <c r="H35">
-        <v>173</v>
+        <v>176.7</v>
       </c>
       <c r="I35">
-        <v>153.1</v>
+        <v>155.9</v>
       </c>
       <c r="J35">
-        <v>117.9</v>
+        <v>120.1</v>
       </c>
       <c r="K35">
-        <v>131.80000000000001</v>
+        <v>133.69999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -1657,34 +1658,34 @@
         <v>44135</v>
       </c>
       <c r="B36">
-        <v>49.4</v>
+        <v>50.7</v>
       </c>
       <c r="C36">
-        <v>67.599999999999994</v>
+        <v>69.400000000000006</v>
       </c>
       <c r="D36">
-        <v>113.8</v>
+        <v>117.1</v>
       </c>
       <c r="E36">
-        <v>162</v>
+        <v>166.7</v>
       </c>
       <c r="F36">
-        <v>234.7</v>
+        <v>228.1</v>
       </c>
       <c r="G36">
-        <v>197.4</v>
+        <v>203.2</v>
       </c>
       <c r="H36">
-        <v>199</v>
+        <v>204.6</v>
       </c>
       <c r="I36">
-        <v>175.2</v>
+        <v>179.2</v>
       </c>
       <c r="J36">
-        <v>131.80000000000001</v>
+        <v>134.69999999999999</v>
       </c>
       <c r="K36">
-        <v>143.30000000000001</v>
+        <v>145.69999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -1692,34 +1693,34 @@
         <v>44142</v>
       </c>
       <c r="B37">
-        <v>65.400000000000006</v>
+        <v>67.099999999999994</v>
       </c>
       <c r="C37">
-        <v>93.6</v>
+        <v>96.4</v>
       </c>
       <c r="D37">
-        <v>162.1</v>
+        <v>167</v>
       </c>
       <c r="E37">
-        <v>242.9</v>
+        <v>250.6</v>
       </c>
       <c r="F37">
-        <v>325.60000000000002</v>
+        <v>321.2</v>
       </c>
       <c r="G37">
-        <v>265.3</v>
+        <v>273.8</v>
       </c>
       <c r="H37">
-        <v>263.5</v>
+        <v>271.10000000000002</v>
       </c>
       <c r="I37">
-        <v>226.1</v>
+        <v>231.8</v>
       </c>
       <c r="J37">
-        <v>170.9</v>
+        <v>174.6</v>
       </c>
       <c r="K37">
-        <v>183.5</v>
+        <v>187</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -1727,34 +1728,34 @@
         <v>44149</v>
       </c>
       <c r="B38">
-        <v>79.8</v>
+        <v>82</v>
       </c>
       <c r="C38">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D38">
-        <v>194.3</v>
+        <v>199.8</v>
       </c>
       <c r="E38">
-        <v>282.10000000000002</v>
+        <v>290.8</v>
       </c>
       <c r="F38">
-        <v>378.2</v>
+        <v>367.9</v>
       </c>
       <c r="G38">
-        <v>313</v>
+        <v>322.60000000000002</v>
       </c>
       <c r="H38">
-        <v>316.5</v>
+        <v>325.3</v>
       </c>
       <c r="I38">
-        <v>277</v>
+        <v>283.60000000000002</v>
       </c>
       <c r="J38">
-        <v>213.2</v>
+        <v>217.9</v>
       </c>
       <c r="K38">
-        <v>227.1</v>
+        <v>231.4</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -1762,34 +1763,34 @@
         <v>44156</v>
       </c>
       <c r="B39">
-        <v>92.5</v>
+        <v>93.6</v>
       </c>
       <c r="C39">
-        <v>129.6</v>
+        <v>131.19999999999999</v>
       </c>
       <c r="D39">
-        <v>213</v>
+        <v>215.8</v>
       </c>
       <c r="E39">
-        <v>299.8</v>
+        <v>303.7</v>
       </c>
       <c r="F39">
-        <v>405.3</v>
+        <v>408.8</v>
       </c>
       <c r="G39">
-        <v>363.9</v>
+        <v>367.7</v>
       </c>
       <c r="H39">
-        <v>362.5</v>
+        <v>366.5</v>
       </c>
       <c r="I39">
-        <v>320.2</v>
+        <v>323.3</v>
       </c>
       <c r="J39">
-        <v>246.1</v>
+        <v>248.4</v>
       </c>
       <c r="K39">
-        <v>270.2</v>
+        <v>272.39999999999998</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -1797,34 +1798,34 @@
         <v>44163</v>
       </c>
       <c r="B40">
-        <v>86.6</v>
+        <v>86.9</v>
       </c>
       <c r="C40">
-        <v>117.2</v>
+        <v>118.3</v>
       </c>
       <c r="D40">
-        <v>189.1</v>
+        <v>190.5</v>
       </c>
       <c r="E40">
-        <v>272.2</v>
+        <v>274.2</v>
       </c>
       <c r="F40">
-        <v>363.1</v>
+        <v>365</v>
       </c>
       <c r="G40">
-        <v>341.1</v>
+        <v>342.9</v>
       </c>
       <c r="H40">
-        <v>342.7</v>
+        <v>344.5</v>
       </c>
       <c r="I40">
-        <v>304.8</v>
+        <v>306.5</v>
       </c>
       <c r="J40">
-        <v>235</v>
+        <v>236.3</v>
       </c>
       <c r="K40">
-        <v>270.8</v>
+        <v>272.5</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -1835,31 +1836,31 @@
         <v>118.2</v>
       </c>
       <c r="C41">
-        <v>164.3</v>
+        <v>164.4</v>
       </c>
       <c r="D41">
-        <v>254.3</v>
+        <v>254.2</v>
       </c>
       <c r="E41">
-        <v>362.1</v>
+        <v>360.9</v>
       </c>
       <c r="F41">
-        <v>471</v>
+        <v>466.2</v>
       </c>
       <c r="G41">
-        <v>436.1</v>
+        <v>431.9</v>
       </c>
       <c r="H41">
-        <v>429.7</v>
+        <v>425.3</v>
       </c>
       <c r="I41">
-        <v>373</v>
+        <v>368.4</v>
       </c>
       <c r="J41">
-        <v>277.60000000000002</v>
+        <v>276.2</v>
       </c>
       <c r="K41">
-        <v>317.60000000000002</v>
+        <v>315.3</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -1867,34 +1868,34 @@
         <v>44177</v>
       </c>
       <c r="B42">
-        <v>123.7</v>
+        <v>124.1</v>
       </c>
       <c r="C42">
-        <v>166.6</v>
+        <v>167.8</v>
       </c>
       <c r="D42">
-        <v>257.39999999999998</v>
+        <v>259.10000000000002</v>
       </c>
       <c r="E42">
-        <v>350.8</v>
+        <v>353.5</v>
       </c>
       <c r="F42">
-        <v>453.1</v>
+        <v>455.6</v>
       </c>
       <c r="G42">
-        <v>430.7</v>
+        <v>433.6</v>
       </c>
       <c r="H42">
-        <v>428.7</v>
+        <v>431</v>
       </c>
       <c r="I42">
-        <v>376.1</v>
+        <v>378.2</v>
       </c>
       <c r="J42">
-        <v>283.3</v>
+        <v>285.3</v>
       </c>
       <c r="K42">
-        <v>322.89999999999998</v>
+        <v>325</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -1902,34 +1903,34 @@
         <v>44184</v>
       </c>
       <c r="B43">
-        <v>119.3</v>
+        <v>119.7</v>
       </c>
       <c r="C43">
-        <v>158.80000000000001</v>
+        <v>159.6</v>
       </c>
       <c r="D43">
-        <v>247.2</v>
+        <v>248.9</v>
       </c>
       <c r="E43">
-        <v>330.7</v>
+        <v>332.3</v>
       </c>
       <c r="F43">
-        <v>425.2</v>
+        <v>427</v>
       </c>
       <c r="G43">
-        <v>413.8</v>
+        <v>415.5</v>
       </c>
       <c r="H43">
-        <v>415.6</v>
+        <v>417.5</v>
       </c>
       <c r="I43">
-        <v>366.7</v>
+        <v>368.5</v>
       </c>
       <c r="J43">
-        <v>275.3</v>
+        <v>277</v>
       </c>
       <c r="K43">
-        <v>311.60000000000002</v>
+        <v>313.5</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -1937,34 +1938,34 @@
         <v>44191</v>
       </c>
       <c r="B44">
-        <v>107.5</v>
+        <v>107.7</v>
       </c>
       <c r="C44">
-        <v>137.30000000000001</v>
+        <v>137.69999999999999</v>
       </c>
       <c r="D44">
-        <v>216.8</v>
+        <v>217.7</v>
       </c>
       <c r="E44">
-        <v>304.8</v>
+        <v>305.89999999999998</v>
       </c>
       <c r="F44">
-        <v>406.3</v>
+        <v>406.8</v>
       </c>
       <c r="G44">
-        <v>398.5</v>
+        <v>399.4</v>
       </c>
       <c r="H44">
-        <v>402.4</v>
+        <v>403.5</v>
       </c>
       <c r="I44">
-        <v>364.6</v>
+        <v>365.8</v>
       </c>
       <c r="J44">
-        <v>285.60000000000002</v>
+        <v>286.7</v>
       </c>
       <c r="K44">
-        <v>315.7</v>
+        <v>317.10000000000002</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
@@ -1972,34 +1973,34 @@
         <v>44198</v>
       </c>
       <c r="B45">
-        <v>126.8</v>
+        <v>128</v>
       </c>
       <c r="C45">
-        <v>169.9</v>
+        <v>171.6</v>
       </c>
       <c r="D45">
-        <v>260.8</v>
+        <v>263.60000000000002</v>
       </c>
       <c r="E45">
-        <v>360.1</v>
+        <v>363.9</v>
       </c>
       <c r="F45">
-        <v>491.9</v>
+        <v>495.9</v>
       </c>
       <c r="G45">
-        <v>468.2</v>
+        <v>472.4</v>
       </c>
       <c r="H45">
-        <v>459.8</v>
+        <v>463.9</v>
       </c>
       <c r="I45">
-        <v>406.5</v>
+        <v>410.3</v>
       </c>
       <c r="J45">
-        <v>314.5</v>
+        <v>317.89999999999998</v>
       </c>
       <c r="K45">
-        <v>341</v>
+        <v>344.1</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -2007,34 +2008,34 @@
         <v>44205</v>
       </c>
       <c r="B46">
-        <v>147.1</v>
+        <v>145</v>
       </c>
       <c r="C46">
-        <v>208.5</v>
+        <v>206</v>
       </c>
       <c r="D46">
-        <v>317.10000000000002</v>
+        <v>312.39999999999998</v>
       </c>
       <c r="E46">
-        <v>440.3</v>
+        <v>432.9</v>
       </c>
       <c r="F46">
-        <v>571.4</v>
+        <v>563</v>
       </c>
       <c r="G46">
-        <v>509.9</v>
+        <v>500.6</v>
       </c>
       <c r="H46">
-        <v>500.7</v>
+        <v>492.1</v>
       </c>
       <c r="I46">
-        <v>440.2</v>
+        <v>432.5</v>
       </c>
       <c r="J46">
-        <v>333.2</v>
+        <v>326.2</v>
       </c>
       <c r="K46">
-        <v>359.8</v>
+        <v>352.1</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
@@ -2042,34 +2043,34 @@
         <v>44212</v>
       </c>
       <c r="B47">
-        <v>127.9</v>
+        <v>128</v>
       </c>
       <c r="C47">
-        <v>171.7</v>
+        <v>171.9</v>
       </c>
       <c r="D47">
-        <v>251.3</v>
+        <v>251.4</v>
       </c>
       <c r="E47">
-        <v>335.8</v>
+        <v>335.9</v>
       </c>
       <c r="F47">
-        <v>422.6</v>
+        <v>422.5</v>
       </c>
       <c r="G47">
-        <v>379.3</v>
+        <v>379.1</v>
       </c>
       <c r="H47">
-        <v>380.3</v>
+        <v>380.5</v>
       </c>
       <c r="I47">
-        <v>344.9</v>
+        <v>344.4</v>
       </c>
       <c r="J47">
-        <v>265.3</v>
+        <v>265.10000000000002</v>
       </c>
       <c r="K47">
-        <v>286.60000000000002</v>
+        <v>286.39999999999998</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
@@ -2083,28 +2084,28 @@
         <v>144.19999999999999</v>
       </c>
       <c r="D48">
-        <v>211.7</v>
+        <v>211.5</v>
       </c>
       <c r="E48">
-        <v>274.3</v>
+        <v>274.10000000000002</v>
       </c>
       <c r="F48">
-        <v>325.5</v>
+        <v>325.3</v>
       </c>
       <c r="G48">
-        <v>300.8</v>
+        <v>300.39999999999998</v>
       </c>
       <c r="H48">
-        <v>302.60000000000002</v>
+        <v>301.7</v>
       </c>
       <c r="I48">
-        <v>273.60000000000002</v>
+        <v>272.60000000000002</v>
       </c>
       <c r="J48">
-        <v>210.7</v>
+        <v>209.6</v>
       </c>
       <c r="K48">
-        <v>226.5</v>
+        <v>226.3</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
@@ -2112,34 +2113,34 @@
         <v>44226</v>
       </c>
       <c r="B49">
-        <v>95.7</v>
+        <v>95.8</v>
       </c>
       <c r="C49">
-        <v>131.4</v>
+        <v>131.6</v>
       </c>
       <c r="D49">
-        <v>194.3</v>
+        <v>194.4</v>
       </c>
       <c r="E49">
-        <v>249.2</v>
+        <v>249.4</v>
       </c>
       <c r="F49">
-        <v>303</v>
+        <v>303.10000000000002</v>
       </c>
       <c r="G49">
-        <v>276.89999999999998</v>
+        <v>276.7</v>
       </c>
       <c r="H49">
-        <v>274</v>
+        <v>273.8</v>
       </c>
       <c r="I49">
-        <v>247</v>
+        <v>246.9</v>
       </c>
       <c r="J49">
         <v>188.5</v>
       </c>
       <c r="K49">
-        <v>198.5</v>
+        <v>198.3</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
@@ -2147,31 +2148,31 @@
         <v>44233</v>
       </c>
       <c r="B50">
-        <v>71.099999999999994</v>
+        <v>71.2</v>
       </c>
       <c r="C50">
-        <v>99</v>
+        <v>99.3</v>
       </c>
       <c r="D50">
-        <v>147.6</v>
+        <v>148.1</v>
       </c>
       <c r="E50">
-        <v>185.7</v>
+        <v>185.9</v>
       </c>
       <c r="F50">
-        <v>211.7</v>
+        <v>211.9</v>
       </c>
       <c r="G50">
-        <v>192.5</v>
+        <v>192.3</v>
       </c>
       <c r="H50">
-        <v>191.4</v>
+        <v>191.3</v>
       </c>
       <c r="I50">
-        <v>172.7</v>
+        <v>172.5</v>
       </c>
       <c r="J50">
-        <v>133.19999999999999</v>
+        <v>133.30000000000001</v>
       </c>
       <c r="K50">
         <v>137.4</v>
@@ -2185,31 +2186,31 @@
         <v>61</v>
       </c>
       <c r="C51">
-        <v>85.5</v>
+        <v>85.7</v>
       </c>
       <c r="D51">
-        <v>125.2</v>
+        <v>125.3</v>
       </c>
       <c r="E51">
-        <v>154.19999999999999</v>
+        <v>154.30000000000001</v>
       </c>
       <c r="F51">
-        <v>184.2</v>
+        <v>184.8</v>
       </c>
       <c r="G51">
-        <v>164.9</v>
+        <v>165</v>
       </c>
       <c r="H51">
-        <v>163.30000000000001</v>
+        <v>163.4</v>
       </c>
       <c r="I51">
-        <v>147.1</v>
+        <v>147</v>
       </c>
       <c r="J51">
         <v>110.3</v>
       </c>
       <c r="K51">
-        <v>111</v>
+        <v>111.2</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
@@ -2217,31 +2218,31 @@
         <v>44247</v>
       </c>
       <c r="B52">
-        <v>49.3</v>
+        <v>49.4</v>
       </c>
       <c r="C52">
-        <v>67.400000000000006</v>
+        <v>67.7</v>
       </c>
       <c r="D52">
-        <v>98.5</v>
+        <v>98.8</v>
       </c>
       <c r="E52">
-        <v>130.19999999999999</v>
+        <v>130.80000000000001</v>
       </c>
       <c r="F52">
-        <v>154.80000000000001</v>
+        <v>155.30000000000001</v>
       </c>
       <c r="G52">
-        <v>134.4</v>
+        <v>134.5</v>
       </c>
       <c r="H52">
-        <v>132.5</v>
+        <v>132.6</v>
       </c>
       <c r="I52">
-        <v>118.9</v>
+        <v>119</v>
       </c>
       <c r="J52">
-        <v>86.4</v>
+        <v>86.3</v>
       </c>
       <c r="K52">
         <v>83.8</v>
@@ -2252,34 +2253,34 @@
         <v>44254</v>
       </c>
       <c r="B53">
-        <v>48.7</v>
+        <v>48.8</v>
       </c>
       <c r="C53">
-        <v>67.3</v>
+        <v>67.400000000000006</v>
       </c>
       <c r="D53">
-        <v>99.7</v>
+        <v>99.8</v>
       </c>
       <c r="E53">
-        <v>128.6</v>
+        <v>128.69999999999999</v>
       </c>
       <c r="F53">
-        <v>155</v>
+        <v>155.4</v>
       </c>
       <c r="G53">
-        <v>132.6</v>
+        <v>132.69999999999999</v>
       </c>
       <c r="H53">
-        <v>126.7</v>
+        <v>126.8</v>
       </c>
       <c r="I53">
         <v>114.6</v>
       </c>
       <c r="J53">
-        <v>82.5</v>
+        <v>82.3</v>
       </c>
       <c r="K53">
-        <v>74.900000000000006</v>
+        <v>75.099999999999994</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -2287,34 +2288,34 @@
         <v>44261</v>
       </c>
       <c r="B54">
-        <v>45.4</v>
+        <v>45.5</v>
       </c>
       <c r="C54">
-        <v>61.3</v>
+        <v>61.4</v>
       </c>
       <c r="D54">
         <v>91.9</v>
       </c>
       <c r="E54">
-        <v>121.6</v>
+        <v>121.1</v>
       </c>
       <c r="F54">
-        <v>138.69999999999999</v>
+        <v>138.80000000000001</v>
       </c>
       <c r="G54">
-        <v>130.5</v>
+        <v>130.30000000000001</v>
       </c>
       <c r="H54">
-        <v>129.9</v>
+        <v>129.69999999999999</v>
       </c>
       <c r="I54">
-        <v>114.9</v>
+        <v>114.7</v>
       </c>
       <c r="J54">
-        <v>74.5</v>
+        <v>74.3</v>
       </c>
       <c r="K54">
-        <v>66.099999999999994</v>
+        <v>65.900000000000006</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -2322,34 +2323,34 @@
         <v>44268</v>
       </c>
       <c r="B55">
-        <v>46.2</v>
+        <v>45.8</v>
       </c>
       <c r="C55">
-        <v>66.2</v>
+        <v>66</v>
       </c>
       <c r="D55">
-        <v>97.2</v>
+        <v>96.2</v>
       </c>
       <c r="E55">
-        <v>129</v>
+        <v>128.30000000000001</v>
       </c>
       <c r="F55">
-        <v>142.9</v>
+        <v>141.80000000000001</v>
       </c>
       <c r="G55">
-        <v>127.2</v>
+        <v>126</v>
       </c>
       <c r="H55">
-        <v>124.7</v>
+        <v>123.7</v>
       </c>
       <c r="I55">
-        <v>110.2</v>
+        <v>109.1</v>
       </c>
       <c r="J55">
-        <v>71.599999999999994</v>
+        <v>70.7</v>
       </c>
       <c r="K55">
-        <v>64.599999999999994</v>
+        <v>63.9</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -2357,34 +2358,34 @@
         <v>44275</v>
       </c>
       <c r="B56">
-        <v>56.7</v>
+        <v>56.9</v>
       </c>
       <c r="C56">
         <v>80.400000000000006</v>
       </c>
       <c r="D56">
-        <v>118.1</v>
+        <v>118.3</v>
       </c>
       <c r="E56">
-        <v>153.69999999999999</v>
+        <v>153.5</v>
       </c>
       <c r="F56">
-        <v>183.1</v>
+        <v>183.4</v>
       </c>
       <c r="G56">
         <v>163.9</v>
       </c>
       <c r="H56">
-        <v>160.1</v>
+        <v>160</v>
       </c>
       <c r="I56">
-        <v>143.5</v>
+        <v>143.4</v>
       </c>
       <c r="J56">
-        <v>94.3</v>
+        <v>94.2</v>
       </c>
       <c r="K56">
-        <v>90.9</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
@@ -2392,34 +2393,34 @@
         <v>44282</v>
       </c>
       <c r="B57">
-        <v>55.5</v>
+        <v>55.8</v>
       </c>
       <c r="C57">
-        <v>80.099999999999994</v>
+        <v>80.599999999999994</v>
       </c>
       <c r="D57">
-        <v>119.7</v>
+        <v>120.2</v>
       </c>
       <c r="E57">
-        <v>158.80000000000001</v>
+        <v>159.80000000000001</v>
       </c>
       <c r="F57">
-        <v>178.7</v>
+        <v>179.9</v>
       </c>
       <c r="G57">
-        <v>154.4</v>
+        <v>155.19999999999999</v>
       </c>
       <c r="H57">
-        <v>145.80000000000001</v>
+        <v>146.5</v>
       </c>
       <c r="I57">
-        <v>126.4</v>
+        <v>127.1</v>
       </c>
       <c r="J57">
-        <v>69.3</v>
+        <v>69.5</v>
       </c>
       <c r="K57">
-        <v>61</v>
+        <v>61.4</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
@@ -2427,34 +2428,34 @@
         <v>44289</v>
       </c>
       <c r="B58">
-        <v>54.1</v>
+        <v>54.2</v>
       </c>
       <c r="C58">
-        <v>73.2</v>
+        <v>73.3</v>
       </c>
       <c r="D58">
         <v>110.1</v>
       </c>
       <c r="E58">
-        <v>148.1</v>
+        <v>147.9</v>
       </c>
       <c r="F58">
-        <v>169.9</v>
+        <v>170.2</v>
       </c>
       <c r="G58">
-        <v>143.9</v>
+        <v>144</v>
       </c>
       <c r="H58">
         <v>134</v>
       </c>
       <c r="I58">
-        <v>111.5</v>
+        <v>111.4</v>
       </c>
       <c r="J58">
-        <v>57.3</v>
+        <v>57.1</v>
       </c>
       <c r="K58">
-        <v>46.9</v>
+        <v>46.8</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -2462,34 +2463,34 @@
         <v>44296</v>
       </c>
       <c r="B59">
-        <v>57.3</v>
+        <v>57.4</v>
       </c>
       <c r="C59">
-        <v>78.900000000000006</v>
+        <v>79.099999999999994</v>
       </c>
       <c r="D59">
-        <v>121.8</v>
+        <v>122</v>
       </c>
       <c r="E59">
-        <v>157.4</v>
+        <v>158</v>
       </c>
       <c r="F59">
-        <v>166.3</v>
+        <v>166.9</v>
       </c>
       <c r="G59">
-        <v>144.19999999999999</v>
+        <v>144.5</v>
       </c>
       <c r="H59">
-        <v>132.4</v>
+        <v>132.6</v>
       </c>
       <c r="I59">
-        <v>108.4</v>
+        <v>108.5</v>
       </c>
       <c r="J59">
-        <v>56.4</v>
+        <v>56.5</v>
       </c>
       <c r="K59">
-        <v>48.9</v>
+        <v>49.2</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -2500,7 +2501,7 @@
         <v>58.9</v>
       </c>
       <c r="C60">
-        <v>83.5</v>
+        <v>83.3</v>
       </c>
       <c r="D60">
         <v>124.5</v>
@@ -2509,22 +2510,22 @@
         <v>158</v>
       </c>
       <c r="F60">
-        <v>162.1</v>
+        <v>162</v>
       </c>
       <c r="G60">
-        <v>141.19999999999999</v>
+        <v>140.9</v>
       </c>
       <c r="H60">
-        <v>126.5</v>
+        <v>126.4</v>
       </c>
       <c r="I60">
-        <v>100.4</v>
+        <v>100.1</v>
       </c>
       <c r="J60">
         <v>53.1</v>
       </c>
       <c r="K60">
-        <v>46.7</v>
+        <v>46.9</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -2538,13 +2539,13 @@
         <v>77.400000000000006</v>
       </c>
       <c r="D61">
-        <v>119.1</v>
+        <v>119.5</v>
       </c>
       <c r="E61">
-        <v>144.69999999999999</v>
+        <v>144.80000000000001</v>
       </c>
       <c r="F61">
-        <v>144.4</v>
+        <v>144.5</v>
       </c>
       <c r="G61">
         <v>127.7</v>
@@ -2559,7 +2560,7 @@
         <v>50.4</v>
       </c>
       <c r="K61">
-        <v>45.2</v>
+        <v>45.3</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -2570,31 +2571,31 @@
         <v>49.4</v>
       </c>
       <c r="C62">
-        <v>70.5</v>
+        <v>70.8</v>
       </c>
       <c r="D62">
-        <v>110.2</v>
+        <v>110.8</v>
       </c>
       <c r="E62">
-        <v>128.5</v>
+        <v>129</v>
       </c>
       <c r="F62">
-        <v>118.3</v>
+        <v>118.8</v>
       </c>
       <c r="G62">
-        <v>107.3</v>
+        <v>107.7</v>
       </c>
       <c r="H62">
-        <v>96.2</v>
+        <v>96.4</v>
       </c>
       <c r="I62">
-        <v>72.7</v>
+        <v>72.8</v>
       </c>
       <c r="J62">
-        <v>42</v>
+        <v>42.2</v>
       </c>
       <c r="K62">
-        <v>36.700000000000003</v>
+        <v>36.9</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
@@ -2602,34 +2603,34 @@
         <v>44324</v>
       </c>
       <c r="B63">
-        <v>45.5</v>
+        <v>45.7</v>
       </c>
       <c r="C63">
-        <v>65.8</v>
+        <v>66.099999999999994</v>
       </c>
       <c r="D63">
-        <v>99.6</v>
+        <v>100.2</v>
       </c>
       <c r="E63">
-        <v>113.1</v>
+        <v>113.7</v>
       </c>
       <c r="F63">
-        <v>109.2</v>
+        <v>109.8</v>
       </c>
       <c r="G63">
-        <v>98.7</v>
+        <v>99.1</v>
       </c>
       <c r="H63">
-        <v>89.6</v>
+        <v>89.9</v>
       </c>
       <c r="I63">
-        <v>69.400000000000006</v>
+        <v>69.599999999999994</v>
       </c>
       <c r="J63">
-        <v>41.2</v>
+        <v>41.4</v>
       </c>
       <c r="K63">
-        <v>36.4</v>
+        <v>36.6</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
@@ -2637,34 +2638,34 @@
         <v>44331</v>
       </c>
       <c r="B64">
-        <v>41.6</v>
+        <v>41.9</v>
       </c>
       <c r="C64">
-        <v>56.5</v>
+        <v>56.9</v>
       </c>
       <c r="D64">
-        <v>86.1</v>
+        <v>86.8</v>
       </c>
       <c r="E64">
-        <v>97</v>
+        <v>97.7</v>
       </c>
       <c r="F64">
-        <v>101.6</v>
+        <v>102.2</v>
       </c>
       <c r="G64">
-        <v>88.7</v>
+        <v>89.4</v>
       </c>
       <c r="H64">
-        <v>80.7</v>
+        <v>81.3</v>
       </c>
       <c r="I64">
-        <v>65.7</v>
+        <v>66.2</v>
       </c>
       <c r="J64">
-        <v>40.299999999999997</v>
+        <v>40.5</v>
       </c>
       <c r="K64">
-        <v>36</v>
+        <v>36.200000000000003</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
@@ -2672,34 +2673,34 @@
         <v>44338</v>
       </c>
       <c r="B65">
-        <v>24.9</v>
+        <v>25.3</v>
       </c>
       <c r="C65">
-        <v>33.1</v>
+        <v>33.5</v>
       </c>
       <c r="D65">
-        <v>52</v>
+        <v>52.4</v>
       </c>
       <c r="E65">
-        <v>55.8</v>
+        <v>56.3</v>
       </c>
       <c r="F65">
-        <v>59.6</v>
+        <v>60.3</v>
       </c>
       <c r="G65">
-        <v>57.6</v>
+        <v>58.2</v>
       </c>
       <c r="H65">
-        <v>52.1</v>
+        <v>52.5</v>
       </c>
       <c r="I65">
-        <v>40.799999999999997</v>
+        <v>41.2</v>
       </c>
       <c r="J65">
-        <v>25.6</v>
+        <v>25.8</v>
       </c>
       <c r="K65">
-        <v>24.5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
@@ -2707,34 +2708,34 @@
         <v>44345</v>
       </c>
       <c r="B66">
-        <v>18</v>
+        <v>18.2</v>
       </c>
       <c r="C66">
-        <v>22.9</v>
+        <v>23.1</v>
       </c>
       <c r="D66">
-        <v>34.4</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="E66">
-        <v>39.299999999999997</v>
+        <v>39.5</v>
       </c>
       <c r="F66">
-        <v>41.5</v>
+        <v>42.1</v>
       </c>
       <c r="G66">
-        <v>40</v>
+        <v>40.6</v>
       </c>
       <c r="H66">
-        <v>35.4</v>
+        <v>35.9</v>
       </c>
       <c r="I66">
-        <v>28.9</v>
+        <v>29.3</v>
       </c>
       <c r="J66">
-        <v>19.7</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="K66">
-        <v>17.899999999999999</v>
+        <v>18.2</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
@@ -2742,34 +2743,34 @@
         <v>44352</v>
       </c>
       <c r="B67">
-        <v>14.3</v>
+        <v>14.5</v>
       </c>
       <c r="C67">
-        <v>16.100000000000001</v>
+        <v>16.5</v>
       </c>
       <c r="D67">
-        <v>23.3</v>
+        <v>23.8</v>
       </c>
       <c r="E67">
-        <v>28.7</v>
+        <v>29.4</v>
       </c>
       <c r="F67">
-        <v>31</v>
+        <v>31.7</v>
       </c>
       <c r="G67">
-        <v>30.2</v>
+        <v>30.9</v>
       </c>
       <c r="H67">
-        <v>27</v>
+        <v>27.7</v>
       </c>
       <c r="I67">
-        <v>21.1</v>
+        <v>21.6</v>
       </c>
       <c r="J67">
-        <v>14.3</v>
+        <v>14.8</v>
       </c>
       <c r="K67">
-        <v>14</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
@@ -2777,34 +2778,34 @@
         <v>44359</v>
       </c>
       <c r="B68">
-        <v>14.6</v>
+        <v>14.9</v>
       </c>
       <c r="C68">
-        <v>17.2</v>
+        <v>17.3</v>
       </c>
       <c r="D68">
-        <v>24.4</v>
+        <v>24.6</v>
       </c>
       <c r="E68">
-        <v>30.4</v>
+        <v>30.6</v>
       </c>
       <c r="F68">
-        <v>36.4</v>
+        <v>37</v>
       </c>
       <c r="G68">
-        <v>35.9</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="H68">
-        <v>31.3</v>
+        <v>31.7</v>
       </c>
       <c r="I68">
-        <v>25</v>
+        <v>25.3</v>
       </c>
       <c r="J68">
-        <v>16.399999999999999</v>
+        <v>16.7</v>
       </c>
       <c r="K68">
-        <v>16.3</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
@@ -2812,34 +2813,34 @@
         <v>44366</v>
       </c>
       <c r="B69">
-        <v>12.4</v>
+        <v>12.7</v>
       </c>
       <c r="C69">
-        <v>14.3</v>
+        <v>14.5</v>
       </c>
       <c r="D69">
-        <v>20</v>
+        <v>20.3</v>
       </c>
       <c r="E69">
-        <v>26</v>
+        <v>26.4</v>
       </c>
       <c r="F69">
-        <v>35.299999999999997</v>
+        <v>35.9</v>
       </c>
       <c r="G69">
-        <v>32</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="H69">
-        <v>28.6</v>
+        <v>29.2</v>
       </c>
       <c r="I69">
-        <v>23.4</v>
+        <v>23.8</v>
       </c>
       <c r="J69">
-        <v>16.7</v>
+        <v>17</v>
       </c>
       <c r="K69">
-        <v>17.2</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
@@ -2847,34 +2848,34 @@
         <v>44373</v>
       </c>
       <c r="B70">
-        <v>12.8</v>
+        <v>13</v>
       </c>
       <c r="C70">
-        <v>15.6</v>
+        <v>15.9</v>
       </c>
       <c r="D70">
-        <v>21.3</v>
+        <v>21.6</v>
       </c>
       <c r="E70">
-        <v>28.3</v>
+        <v>28.8</v>
       </c>
       <c r="F70">
-        <v>36.5</v>
+        <v>37</v>
       </c>
       <c r="G70">
-        <v>32.700000000000003</v>
+        <v>33</v>
       </c>
       <c r="H70">
-        <v>28.4</v>
+        <v>28.8</v>
       </c>
       <c r="I70">
-        <v>22.4</v>
+        <v>22.6</v>
       </c>
       <c r="J70">
-        <v>15.8</v>
+        <v>16</v>
       </c>
       <c r="K70">
-        <v>14</v>
+        <v>14.3</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
@@ -2882,34 +2883,34 @@
         <v>44380</v>
       </c>
       <c r="B71">
-        <v>16.3</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="C71">
-        <v>20.100000000000001</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="D71">
-        <v>28.6</v>
+        <v>29</v>
       </c>
       <c r="E71">
-        <v>34.9</v>
+        <v>35.5</v>
       </c>
       <c r="F71">
-        <v>44.2</v>
+        <v>44.8</v>
       </c>
       <c r="G71">
-        <v>41.9</v>
+        <v>42.5</v>
       </c>
       <c r="H71">
-        <v>36.200000000000003</v>
+        <v>36.6</v>
       </c>
       <c r="I71">
-        <v>27</v>
+        <v>27.4</v>
       </c>
       <c r="J71">
-        <v>18</v>
+        <v>18.3</v>
       </c>
       <c r="K71">
-        <v>16.8</v>
+        <v>17.100000000000001</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
@@ -2917,34 +2918,34 @@
         <v>44387</v>
       </c>
       <c r="B72">
-        <v>20.7</v>
+        <v>21.1</v>
       </c>
       <c r="C72">
-        <v>28.8</v>
+        <v>29.3</v>
       </c>
       <c r="D72">
-        <v>36.6</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="E72">
-        <v>47.6</v>
+        <v>48.4</v>
       </c>
       <c r="F72">
-        <v>62.9</v>
+        <v>63.9</v>
       </c>
       <c r="G72">
-        <v>59.4</v>
+        <v>60.4</v>
       </c>
       <c r="H72">
-        <v>49.7</v>
+        <v>50.5</v>
       </c>
       <c r="I72">
-        <v>36.4</v>
+        <v>37.1</v>
       </c>
       <c r="J72">
-        <v>24.5</v>
+        <v>25.1</v>
       </c>
       <c r="K72">
-        <v>21.8</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
@@ -2987,34 +2988,34 @@
         <v>44401</v>
       </c>
       <c r="B74">
-        <v>45.1</v>
+        <v>46.3</v>
       </c>
       <c r="C74">
-        <v>63.9</v>
+        <v>65.7</v>
       </c>
       <c r="D74">
-        <v>75.900000000000006</v>
+        <v>78.099999999999994</v>
       </c>
       <c r="E74">
-        <v>97.2</v>
+        <v>99.6</v>
       </c>
       <c r="F74">
-        <v>122.2</v>
+        <v>124.8</v>
       </c>
       <c r="G74">
-        <v>118.3</v>
+        <v>121.3</v>
       </c>
       <c r="H74">
-        <v>96.6</v>
+        <v>99.2</v>
       </c>
       <c r="I74">
-        <v>68.8</v>
+        <v>71</v>
       </c>
       <c r="J74">
-        <v>48.7</v>
+        <v>50.8</v>
       </c>
       <c r="K74">
-        <v>41.1</v>
+        <v>42.8</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
@@ -3022,34 +3023,34 @@
         <v>44408</v>
       </c>
       <c r="B75">
-        <v>67.900000000000006</v>
+        <v>70.5</v>
       </c>
       <c r="C75">
-        <v>97.4</v>
+        <v>102</v>
       </c>
       <c r="D75">
-        <v>110</v>
+        <v>114.9</v>
       </c>
       <c r="E75">
-        <v>137.1</v>
+        <v>143.1</v>
       </c>
       <c r="F75">
-        <v>175.2</v>
+        <v>181.1</v>
       </c>
       <c r="G75">
-        <v>164.9</v>
+        <v>171.6</v>
       </c>
       <c r="H75">
-        <v>136.30000000000001</v>
+        <v>142.1</v>
       </c>
       <c r="I75">
-        <v>96.2</v>
+        <v>100.7</v>
       </c>
       <c r="J75">
-        <v>69.099999999999994</v>
+        <v>73.2</v>
       </c>
       <c r="K75">
-        <v>61.5</v>
+        <v>64.8</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
@@ -3057,34 +3058,34 @@
         <v>44415</v>
       </c>
       <c r="B76">
-        <v>83.3</v>
+        <v>95.7</v>
       </c>
       <c r="C76">
-        <v>118.5</v>
+        <v>137.6</v>
       </c>
       <c r="D76">
-        <v>130.69999999999999</v>
+        <v>154.9</v>
       </c>
       <c r="E76">
-        <v>158.9</v>
+        <v>188.6</v>
       </c>
       <c r="F76">
-        <v>197.2</v>
+        <v>234.3</v>
       </c>
       <c r="G76">
-        <v>188.1</v>
+        <v>227.8</v>
       </c>
       <c r="H76">
-        <v>158.4</v>
+        <v>195.5</v>
       </c>
       <c r="I76">
-        <v>114.2</v>
+        <v>145.6</v>
       </c>
       <c r="J76">
-        <v>82.5</v>
+        <v>107.5</v>
       </c>
       <c r="K76">
-        <v>73.7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
@@ -3092,34 +3093,34 @@
         <v>44422</v>
       </c>
       <c r="B77">
-        <v>97.8</v>
+        <v>121.5</v>
       </c>
       <c r="C77">
-        <v>152</v>
+        <v>190.4</v>
       </c>
       <c r="D77">
-        <v>166.1</v>
+        <v>205.4</v>
       </c>
       <c r="E77">
-        <v>193.8</v>
+        <v>239</v>
       </c>
       <c r="F77">
-        <v>213.2</v>
+        <v>254.3</v>
       </c>
       <c r="G77">
-        <v>208.4</v>
+        <v>254.2</v>
       </c>
       <c r="H77">
-        <v>178.1</v>
+        <v>219.5</v>
       </c>
       <c r="I77">
-        <v>129.4</v>
+        <v>161.4</v>
       </c>
       <c r="J77">
-        <v>93.9</v>
+        <v>120.6</v>
       </c>
       <c r="K77">
-        <v>85.8</v>
+        <v>109.3</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
@@ -3127,34 +3128,34 @@
         <v>44429</v>
       </c>
       <c r="B78">
-        <v>52.5</v>
+        <v>129.1</v>
       </c>
       <c r="C78">
-        <v>87.7</v>
+        <v>227.7</v>
       </c>
       <c r="D78">
-        <v>99.7</v>
+        <v>251.3</v>
       </c>
       <c r="E78">
-        <v>105.9</v>
+        <v>263.7</v>
       </c>
       <c r="F78">
-        <v>99.8</v>
+        <v>238.9</v>
       </c>
       <c r="G78">
-        <v>101.1</v>
+        <v>244.4</v>
       </c>
       <c r="H78">
-        <v>87</v>
+        <v>209.1</v>
       </c>
       <c r="I78">
-        <v>64.3</v>
+        <v>156</v>
       </c>
       <c r="J78">
-        <v>47.8</v>
+        <v>120.9</v>
       </c>
       <c r="K78">
-        <v>42.8</v>
+        <v>107.6</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
@@ -3162,34 +3163,34 @@
         <v>44436</v>
       </c>
       <c r="B79">
-        <v>70.599999999999994</v>
+        <v>158.9</v>
       </c>
       <c r="C79">
-        <v>120.8</v>
+        <v>284.10000000000002</v>
       </c>
       <c r="D79">
-        <v>141.6</v>
+        <v>327.9</v>
       </c>
       <c r="E79">
-        <v>148.1</v>
+        <v>341.3</v>
       </c>
       <c r="F79">
-        <v>136.80000000000001</v>
+        <v>291</v>
       </c>
       <c r="G79">
-        <v>138.30000000000001</v>
+        <v>293.60000000000002</v>
       </c>
       <c r="H79">
-        <v>119.7</v>
+        <v>252.1</v>
       </c>
       <c r="I79">
-        <v>90</v>
+        <v>188.4</v>
       </c>
       <c r="J79">
-        <v>66.599999999999994</v>
+        <v>142.6</v>
       </c>
       <c r="K79">
-        <v>60.6</v>
+        <v>126.8</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
@@ -3197,34 +3198,34 @@
         <v>44443</v>
       </c>
       <c r="B80">
-        <v>121.1</v>
+        <v>132.6</v>
       </c>
       <c r="C80">
-        <v>228.1</v>
+        <v>252.8</v>
       </c>
       <c r="D80">
-        <v>264.5</v>
+        <v>294</v>
       </c>
       <c r="E80">
-        <v>274.2</v>
+        <v>305.10000000000002</v>
       </c>
       <c r="F80">
-        <v>218.6</v>
+        <v>238.1</v>
       </c>
       <c r="G80">
-        <v>223.1</v>
+        <v>244.2</v>
       </c>
       <c r="H80">
-        <v>192</v>
+        <v>211.4</v>
       </c>
       <c r="I80">
-        <v>142.9</v>
+        <v>157.80000000000001</v>
       </c>
       <c r="J80">
-        <v>109.3</v>
+        <v>122.2</v>
       </c>
       <c r="K80">
-        <v>99.1</v>
+        <v>110.3</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
@@ -3232,35 +3233,118 @@
         <v>44450</v>
       </c>
       <c r="B81">
-        <v>89.6</v>
+        <v>126.2</v>
       </c>
       <c r="C81">
-        <v>165.7</v>
+        <v>235.6</v>
       </c>
       <c r="D81">
-        <v>192.3</v>
+        <v>276.89999999999998</v>
       </c>
       <c r="E81">
-        <v>198.8</v>
+        <v>289.5</v>
       </c>
       <c r="F81">
-        <v>162.1</v>
+        <v>230.6</v>
       </c>
       <c r="G81">
-        <v>166.1</v>
+        <v>237.5</v>
       </c>
       <c r="H81">
-        <v>145.80000000000001</v>
+        <v>207.9</v>
       </c>
       <c r="I81">
+        <v>155.5</v>
+      </c>
+      <c r="J81">
+        <v>119.9</v>
+      </c>
+      <c r="K81">
         <v>109.1</v>
       </c>
-      <c r="J81">
-        <v>82.8</v>
-      </c>
-      <c r="K81">
-        <v>75.5</v>
-      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>44457</v>
+      </c>
+      <c r="B82">
+        <v>138.9</v>
+      </c>
+      <c r="C82">
+        <v>243.5</v>
+      </c>
+      <c r="D82">
+        <v>266.3</v>
+      </c>
+      <c r="E82">
+        <v>284.10000000000002</v>
+      </c>
+      <c r="F82">
+        <v>250.2</v>
+      </c>
+      <c r="G82">
+        <v>261.60000000000002</v>
+      </c>
+      <c r="H82">
+        <v>231.7</v>
+      </c>
+      <c r="I82">
+        <v>179</v>
+      </c>
+      <c r="J82">
+        <v>138.80000000000001</v>
+      </c>
+      <c r="K82">
+        <v>127.7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A83" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4571D5CF-E411-3B4E-8AAF-5136E7E11E59}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated rate data from CDC
</commit_message>
<xml_diff>
--- a/case_data.xlsx
+++ b/case_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timwiemken/Library/Mobile Documents/com~apple~CloudDocs/Work/Pfizer/COVID pediatric case count/count github/covid-agegroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A64667D-6D84-8842-859F-077D40D08BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4F877F-E101-504B-8524-CE8901A1BA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="500" windowWidth="27600" windowHeight="17500" xr2:uid="{CC2C058F-5A66-1E4E-8340-2D9DC2FB7952}"/>
   </bookViews>
@@ -422,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14FFA509-206F-304C-A5FE-F366C177BBC6}">
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3058,34 +3058,34 @@
         <v>44415</v>
       </c>
       <c r="B76">
-        <v>95.7</v>
+        <v>96.1</v>
       </c>
       <c r="C76">
-        <v>137.6</v>
+        <v>138</v>
       </c>
       <c r="D76">
-        <v>154.9</v>
+        <v>155.30000000000001</v>
       </c>
       <c r="E76">
-        <v>188.6</v>
+        <v>189.2</v>
       </c>
       <c r="F76">
-        <v>234.3</v>
+        <v>234.9</v>
       </c>
       <c r="G76">
-        <v>227.8</v>
+        <v>228.8</v>
       </c>
       <c r="H76">
-        <v>195.5</v>
+        <v>196.4</v>
       </c>
       <c r="I76">
-        <v>145.6</v>
+        <v>146.30000000000001</v>
       </c>
       <c r="J76">
-        <v>107.5</v>
+        <v>108.3</v>
       </c>
       <c r="K76">
-        <v>103</v>
+        <v>103.7</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
@@ -3093,34 +3093,34 @@
         <v>44422</v>
       </c>
       <c r="B77">
-        <v>121.5</v>
+        <v>122.5</v>
       </c>
       <c r="C77">
-        <v>190.4</v>
+        <v>192.1</v>
       </c>
       <c r="D77">
-        <v>205.4</v>
+        <v>207.3</v>
       </c>
       <c r="E77">
-        <v>239</v>
+        <v>241.2</v>
       </c>
       <c r="F77">
-        <v>254.3</v>
+        <v>255.5</v>
       </c>
       <c r="G77">
-        <v>254.2</v>
+        <v>255.6</v>
       </c>
       <c r="H77">
-        <v>219.5</v>
+        <v>221.1</v>
       </c>
       <c r="I77">
-        <v>161.4</v>
+        <v>162.69999999999999</v>
       </c>
       <c r="J77">
-        <v>120.6</v>
+        <v>121.7</v>
       </c>
       <c r="K77">
-        <v>109.3</v>
+        <v>110.6</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
@@ -3128,34 +3128,34 @@
         <v>44429</v>
       </c>
       <c r="B78">
-        <v>129.1</v>
+        <v>131.6</v>
       </c>
       <c r="C78">
-        <v>227.7</v>
+        <v>233.5</v>
       </c>
       <c r="D78">
-        <v>251.3</v>
+        <v>257.5</v>
       </c>
       <c r="E78">
-        <v>263.7</v>
+        <v>269.7</v>
       </c>
       <c r="F78">
-        <v>238.9</v>
+        <v>241.8</v>
       </c>
       <c r="G78">
-        <v>244.4</v>
+        <v>248.2</v>
       </c>
       <c r="H78">
-        <v>209.1</v>
+        <v>212.4</v>
       </c>
       <c r="I78">
-        <v>156</v>
+        <v>158.6</v>
       </c>
       <c r="J78">
-        <v>120.9</v>
+        <v>123.4</v>
       </c>
       <c r="K78">
-        <v>107.6</v>
+        <v>110.7</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
@@ -3163,34 +3163,34 @@
         <v>44436</v>
       </c>
       <c r="B79">
-        <v>158.9</v>
+        <v>162.5</v>
       </c>
       <c r="C79">
-        <v>284.10000000000002</v>
+        <v>292.8</v>
       </c>
       <c r="D79">
-        <v>327.9</v>
+        <v>337.9</v>
       </c>
       <c r="E79">
-        <v>341.3</v>
+        <v>349.3</v>
       </c>
       <c r="F79">
-        <v>291</v>
+        <v>294.8</v>
       </c>
       <c r="G79">
-        <v>293.60000000000002</v>
+        <v>298.3</v>
       </c>
       <c r="H79">
-        <v>252.1</v>
+        <v>256.2</v>
       </c>
       <c r="I79">
-        <v>188.4</v>
+        <v>191.3</v>
       </c>
       <c r="J79">
-        <v>142.6</v>
+        <v>145.6</v>
       </c>
       <c r="K79">
-        <v>126.8</v>
+        <v>130.1</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
@@ -3198,34 +3198,34 @@
         <v>44443</v>
       </c>
       <c r="B80">
-        <v>132.6</v>
+        <v>136</v>
       </c>
       <c r="C80">
-        <v>252.8</v>
+        <v>259.8</v>
       </c>
       <c r="D80">
-        <v>294</v>
+        <v>301.2</v>
       </c>
       <c r="E80">
-        <v>305.10000000000002</v>
+        <v>312.10000000000002</v>
       </c>
       <c r="F80">
-        <v>238.1</v>
+        <v>242.3</v>
       </c>
       <c r="G80">
-        <v>244.2</v>
+        <v>249.1</v>
       </c>
       <c r="H80">
-        <v>211.4</v>
+        <v>215.9</v>
       </c>
       <c r="I80">
-        <v>157.80000000000001</v>
+        <v>161.30000000000001</v>
       </c>
       <c r="J80">
-        <v>122.2</v>
+        <v>125.2</v>
       </c>
       <c r="K80">
-        <v>110.3</v>
+        <v>113.8</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
@@ -3233,34 +3233,34 @@
         <v>44450</v>
       </c>
       <c r="B81">
-        <v>126.2</v>
+        <v>131.6</v>
       </c>
       <c r="C81">
-        <v>235.6</v>
+        <v>246.2</v>
       </c>
       <c r="D81">
-        <v>276.89999999999998</v>
+        <v>289.2</v>
       </c>
       <c r="E81">
-        <v>289.5</v>
+        <v>302.2</v>
       </c>
       <c r="F81">
-        <v>230.6</v>
+        <v>240.7</v>
       </c>
       <c r="G81">
-        <v>237.5</v>
+        <v>247.9</v>
       </c>
       <c r="H81">
-        <v>207.9</v>
+        <v>217.3</v>
       </c>
       <c r="I81">
-        <v>155.5</v>
+        <v>162.4</v>
       </c>
       <c r="J81">
-        <v>119.9</v>
+        <v>125.3</v>
       </c>
       <c r="K81">
-        <v>109.1</v>
+        <v>114.3</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
@@ -3268,38 +3268,70 @@
         <v>44457</v>
       </c>
       <c r="B82">
-        <v>138.9</v>
+        <v>150</v>
       </c>
       <c r="C82">
-        <v>243.5</v>
+        <v>265.2</v>
       </c>
       <c r="D82">
-        <v>266.3</v>
+        <v>289.2</v>
       </c>
       <c r="E82">
-        <v>284.10000000000002</v>
+        <v>307.10000000000002</v>
       </c>
       <c r="F82">
-        <v>250.2</v>
+        <v>268.2</v>
       </c>
       <c r="G82">
-        <v>261.60000000000002</v>
+        <v>281.7</v>
       </c>
       <c r="H82">
-        <v>231.7</v>
+        <v>250</v>
       </c>
       <c r="I82">
-        <v>179</v>
+        <v>193.1</v>
       </c>
       <c r="J82">
-        <v>138.80000000000001</v>
+        <v>149.69999999999999</v>
       </c>
       <c r="K82">
-        <v>127.7</v>
+        <v>137.4</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A83" s="1"/>
+      <c r="A83" s="1">
+        <v>44464</v>
+      </c>
+      <c r="B83">
+        <v>111.8</v>
+      </c>
+      <c r="C83">
+        <v>202.9</v>
+      </c>
+      <c r="D83">
+        <v>211</v>
+      </c>
+      <c r="E83">
+        <v>219.5</v>
+      </c>
+      <c r="F83">
+        <v>181.7</v>
+      </c>
+      <c r="G83">
+        <v>199.4</v>
+      </c>
+      <c r="H83">
+        <v>177.8</v>
+      </c>
+      <c r="I83">
+        <v>138.1</v>
+      </c>
+      <c r="J83">
+        <v>112.5</v>
+      </c>
+      <c r="K83">
+        <v>104.9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3308,42 +3340,298 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4571D5CF-E411-3B4E-8AAF-5136E7E11E59}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection sqref="A1:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="1">
+        <v>44415</v>
+      </c>
+      <c r="B1">
+        <v>96.1</v>
+      </c>
+      <c r="C1">
+        <v>138</v>
+      </c>
+      <c r="D1">
+        <v>155.30000000000001</v>
+      </c>
+      <c r="E1">
+        <v>189.2</v>
+      </c>
+      <c r="F1">
+        <v>234.9</v>
+      </c>
+      <c r="G1">
+        <v>228.8</v>
+      </c>
+      <c r="H1">
+        <v>196.4</v>
+      </c>
+      <c r="I1">
+        <v>146.30000000000001</v>
+      </c>
+      <c r="J1">
+        <v>108.3</v>
+      </c>
+      <c r="K1">
+        <v>103.7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>44422</v>
+      </c>
+      <c r="B2">
+        <v>122.5</v>
+      </c>
+      <c r="C2">
+        <v>192.1</v>
+      </c>
+      <c r="D2">
+        <v>207.3</v>
+      </c>
+      <c r="E2">
+        <v>241.2</v>
+      </c>
+      <c r="F2">
+        <v>255.5</v>
+      </c>
+      <c r="G2">
+        <v>255.6</v>
+      </c>
+      <c r="H2">
+        <v>221.1</v>
+      </c>
+      <c r="I2">
+        <v>162.69999999999999</v>
+      </c>
+      <c r="J2">
+        <v>121.7</v>
+      </c>
+      <c r="K2">
+        <v>110.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>44429</v>
+      </c>
+      <c r="B3">
+        <v>131.6</v>
+      </c>
+      <c r="C3">
+        <v>233.5</v>
+      </c>
+      <c r="D3">
+        <v>257.5</v>
+      </c>
+      <c r="E3">
+        <v>269.7</v>
+      </c>
+      <c r="F3">
+        <v>241.8</v>
+      </c>
+      <c r="G3">
+        <v>248.2</v>
+      </c>
+      <c r="H3">
+        <v>212.4</v>
+      </c>
+      <c r="I3">
+        <v>158.6</v>
+      </c>
+      <c r="J3">
+        <v>123.4</v>
+      </c>
+      <c r="K3">
+        <v>110.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>44436</v>
+      </c>
+      <c r="B4">
+        <v>162.5</v>
+      </c>
+      <c r="C4">
+        <v>292.8</v>
+      </c>
+      <c r="D4">
+        <v>337.9</v>
+      </c>
+      <c r="E4">
+        <v>349.3</v>
+      </c>
+      <c r="F4">
+        <v>294.8</v>
+      </c>
+      <c r="G4">
+        <v>298.3</v>
+      </c>
+      <c r="H4">
+        <v>256.2</v>
+      </c>
+      <c r="I4">
+        <v>191.3</v>
+      </c>
+      <c r="J4">
+        <v>145.6</v>
+      </c>
+      <c r="K4">
+        <v>130.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>44443</v>
+      </c>
+      <c r="B5">
+        <v>136</v>
+      </c>
+      <c r="C5">
+        <v>259.8</v>
+      </c>
+      <c r="D5">
+        <v>301.2</v>
+      </c>
+      <c r="E5">
+        <v>312.10000000000002</v>
+      </c>
+      <c r="F5">
+        <v>242.3</v>
+      </c>
+      <c r="G5">
+        <v>249.1</v>
+      </c>
+      <c r="H5">
+        <v>215.9</v>
+      </c>
+      <c r="I5">
+        <v>161.30000000000001</v>
+      </c>
+      <c r="J5">
+        <v>125.2</v>
+      </c>
+      <c r="K5">
+        <v>113.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>44450</v>
+      </c>
+      <c r="B6">
+        <v>131.6</v>
+      </c>
+      <c r="C6">
+        <v>246.2</v>
+      </c>
+      <c r="D6">
+        <v>289.2</v>
+      </c>
+      <c r="E6">
+        <v>302.2</v>
+      </c>
+      <c r="F6">
+        <v>240.7</v>
+      </c>
+      <c r="G6">
+        <v>247.9</v>
+      </c>
+      <c r="H6">
+        <v>217.3</v>
+      </c>
+      <c r="I6">
+        <v>162.4</v>
+      </c>
+      <c r="J6">
+        <v>125.3</v>
+      </c>
+      <c r="K6">
+        <v>114.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>44457</v>
+      </c>
+      <c r="B7">
+        <v>150</v>
+      </c>
+      <c r="C7">
+        <v>265.2</v>
+      </c>
+      <c r="D7">
+        <v>289.2</v>
+      </c>
+      <c r="E7">
+        <v>307.10000000000002</v>
+      </c>
+      <c r="F7">
+        <v>268.2</v>
+      </c>
+      <c r="G7">
+        <v>281.7</v>
+      </c>
+      <c r="H7">
+        <v>250</v>
+      </c>
+      <c r="I7">
+        <v>193.1</v>
+      </c>
+      <c r="J7">
+        <v>149.69999999999999</v>
+      </c>
+      <c r="K7">
+        <v>137.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>44464</v>
+      </c>
+      <c r="B8">
+        <v>111.8</v>
+      </c>
+      <c r="C8">
+        <v>202.9</v>
+      </c>
+      <c r="D8">
+        <v>211</v>
+      </c>
+      <c r="E8">
+        <v>219.5</v>
+      </c>
+      <c r="F8">
+        <v>181.7</v>
+      </c>
+      <c r="G8">
+        <v>199.4</v>
+      </c>
+      <c r="H8">
+        <v>177.8</v>
+      </c>
+      <c r="I8">
+        <v>138.1</v>
+      </c>
+      <c r="J8">
+        <v>112.5</v>
+      </c>
+      <c r="K8">
+        <v>104.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update case and hosp nov 12
</commit_message>
<xml_diff>
--- a/case_data.xlsx
+++ b/case_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timwiemken/Library/Mobile Documents/com~apple~CloudDocs/Work/Pfizer/COVID pediatric case count/count github/covid-agegroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81AE6F7-4610-E44E-BAFB-287CBFAE4CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64ED935-E650-9348-B66A-D5737C8B2C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="500" windowWidth="27600" windowHeight="17500" xr2:uid="{CC2C058F-5A66-1E4E-8340-2D9DC2FB7952}"/>
   </bookViews>
@@ -420,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14FFA509-206F-304C-A5FE-F366C177BBC6}">
-  <dimension ref="A1:K87"/>
+  <dimension ref="A1:K88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:K67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,7 +486,7 @@
         <v>2.4</v>
       </c>
       <c r="H2">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="I2">
         <v>4</v>
@@ -518,19 +518,19 @@
         <v>8.5</v>
       </c>
       <c r="G3">
-        <v>12.2</v>
+        <v>12.1</v>
       </c>
       <c r="H3">
-        <v>14.6</v>
+        <v>14.5</v>
       </c>
       <c r="I3">
-        <v>15.3</v>
+        <v>15.2</v>
       </c>
       <c r="J3">
-        <v>13.3</v>
+        <v>13.2</v>
       </c>
       <c r="K3">
-        <v>11.9</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -550,22 +550,22 @@
         <v>6</v>
       </c>
       <c r="F4">
-        <v>30.2</v>
+        <v>30.1</v>
       </c>
       <c r="G4">
-        <v>42.3</v>
+        <v>42.2</v>
       </c>
       <c r="H4">
         <v>48</v>
       </c>
       <c r="I4">
-        <v>49.2</v>
+        <v>49.1</v>
       </c>
       <c r="J4">
-        <v>39.9</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="K4">
-        <v>36.299999999999997</v>
+        <v>36.200000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -591,16 +591,16 @@
         <v>57.1</v>
       </c>
       <c r="H5">
-        <v>65.8</v>
+        <v>65.7</v>
       </c>
       <c r="I5">
-        <v>69.3</v>
+        <v>69.099999999999994</v>
       </c>
       <c r="J5">
-        <v>54.4</v>
+        <v>54.1</v>
       </c>
       <c r="K5">
-        <v>65.400000000000006</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -623,19 +623,19 @@
         <v>43.5</v>
       </c>
       <c r="G6">
-        <v>65.8</v>
+        <v>65.7</v>
       </c>
       <c r="H6">
-        <v>77.599999999999994</v>
+        <v>77.400000000000006</v>
       </c>
       <c r="I6">
-        <v>83.6</v>
+        <v>83.2</v>
       </c>
       <c r="J6">
-        <v>66.3</v>
+        <v>65.599999999999994</v>
       </c>
       <c r="K6">
-        <v>96.9</v>
+        <v>95.1</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -655,22 +655,22 @@
         <v>13.6</v>
       </c>
       <c r="F7">
-        <v>46.1</v>
+        <v>46</v>
       </c>
       <c r="G7">
-        <v>64.8</v>
+        <v>64.7</v>
       </c>
       <c r="H7">
-        <v>77.5</v>
+        <v>77.3</v>
       </c>
       <c r="I7">
-        <v>82.5</v>
+        <v>82.1</v>
       </c>
       <c r="J7">
-        <v>68.099999999999994</v>
+        <v>66.900000000000006</v>
       </c>
       <c r="K7">
-        <v>124.5</v>
+        <v>121.3</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -678,7 +678,7 @@
         <v>43939</v>
       </c>
       <c r="B8">
-        <v>5.7</v>
+        <v>5.6</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -690,22 +690,22 @@
         <v>15</v>
       </c>
       <c r="F8">
-        <v>46.2</v>
+        <v>46.1</v>
       </c>
       <c r="G8">
-        <v>61.3</v>
+        <v>61.1</v>
       </c>
       <c r="H8">
-        <v>69.400000000000006</v>
+        <v>69.2</v>
       </c>
       <c r="I8">
-        <v>71.5</v>
+        <v>71.2</v>
       </c>
       <c r="J8">
-        <v>58.9</v>
+        <v>58.3</v>
       </c>
       <c r="K8">
-        <v>121.3</v>
+        <v>118.5</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -725,22 +725,22 @@
         <v>20.100000000000001</v>
       </c>
       <c r="F9">
-        <v>54.5</v>
+        <v>54.3</v>
       </c>
       <c r="G9">
-        <v>68.099999999999994</v>
+        <v>68</v>
       </c>
       <c r="H9">
-        <v>76</v>
+        <v>75.900000000000006</v>
       </c>
       <c r="I9">
-        <v>72.8</v>
+        <v>72.5</v>
       </c>
       <c r="J9">
-        <v>56.9</v>
+        <v>56.5</v>
       </c>
       <c r="K9">
-        <v>118.6</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -751,7 +751,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="C10">
-        <v>8.6999999999999993</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="D10">
         <v>15</v>
@@ -760,22 +760,22 @@
         <v>25.3</v>
       </c>
       <c r="F10">
-        <v>62</v>
+        <v>61.9</v>
       </c>
       <c r="G10">
-        <v>71.900000000000006</v>
+        <v>71.8</v>
       </c>
       <c r="H10">
-        <v>78.099999999999994</v>
+        <v>78</v>
       </c>
       <c r="I10">
-        <v>70.2</v>
+        <v>70.099999999999994</v>
       </c>
       <c r="J10">
-        <v>52.5</v>
+        <v>52.3</v>
       </c>
       <c r="K10">
-        <v>104.5</v>
+        <v>103.7</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -795,22 +795,22 @@
         <v>26.6</v>
       </c>
       <c r="F11">
-        <v>55.5</v>
+        <v>55.4</v>
       </c>
       <c r="G11">
-        <v>63</v>
+        <v>62.9</v>
       </c>
       <c r="H11">
-        <v>65.099999999999994</v>
+        <v>65</v>
       </c>
       <c r="I11">
-        <v>59.6</v>
+        <v>59.5</v>
       </c>
       <c r="J11">
-        <v>45</v>
+        <v>44.9</v>
       </c>
       <c r="K11">
-        <v>83.8</v>
+        <v>83.3</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -818,7 +818,7 @@
         <v>43967</v>
       </c>
       <c r="B12">
-        <v>12.1</v>
+        <v>12.2</v>
       </c>
       <c r="C12">
         <v>12</v>
@@ -833,19 +833,19 @@
         <v>57.6</v>
       </c>
       <c r="G12">
-        <v>62.7</v>
+        <v>62.6</v>
       </c>
       <c r="H12">
         <v>64.7</v>
       </c>
       <c r="I12">
-        <v>57.6</v>
+        <v>57.5</v>
       </c>
       <c r="J12">
-        <v>42.1</v>
+        <v>42</v>
       </c>
       <c r="K12">
-        <v>77</v>
+        <v>76.7</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -853,7 +853,7 @@
         <v>43974</v>
       </c>
       <c r="B13">
-        <v>13.2</v>
+        <v>13.1</v>
       </c>
       <c r="C13">
         <v>13.3</v>
@@ -877,10 +877,10 @@
         <v>54.5</v>
       </c>
       <c r="J13">
-        <v>39.5</v>
+        <v>39.4</v>
       </c>
       <c r="K13">
-        <v>65.3</v>
+        <v>65.099999999999994</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -915,7 +915,7 @@
         <v>34</v>
       </c>
       <c r="K14">
-        <v>57.8</v>
+        <v>57.5</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -938,19 +938,19 @@
         <v>60.6</v>
       </c>
       <c r="G15">
-        <v>56.8</v>
+        <v>56.7</v>
       </c>
       <c r="H15">
         <v>56.9</v>
       </c>
       <c r="I15">
-        <v>46.2</v>
+        <v>46.1</v>
       </c>
       <c r="J15">
-        <v>32.4</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="K15">
-        <v>49.1</v>
+        <v>48.9</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -979,13 +979,13 @@
         <v>61.8</v>
       </c>
       <c r="I16">
-        <v>48.9</v>
+        <v>48.8</v>
       </c>
       <c r="J16">
         <v>34.700000000000003</v>
       </c>
       <c r="K16">
-        <v>47.1</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1008,19 +1008,19 @@
         <v>110.6</v>
       </c>
       <c r="G17">
-        <v>88.2</v>
+        <v>88.1</v>
       </c>
       <c r="H17">
         <v>82.1</v>
       </c>
       <c r="I17">
-        <v>63.1</v>
+        <v>63</v>
       </c>
       <c r="J17">
-        <v>42.5</v>
+        <v>42.4</v>
       </c>
       <c r="K17">
-        <v>51.5</v>
+        <v>51.4</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -1055,7 +1055,7 @@
         <v>53</v>
       </c>
       <c r="K18">
-        <v>66.900000000000006</v>
+        <v>66.8</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -1081,7 +1081,7 @@
         <v>123.5</v>
       </c>
       <c r="H19">
-        <v>112.9</v>
+        <v>112.8</v>
       </c>
       <c r="I19">
         <v>87.3</v>
@@ -1107,7 +1107,7 @@
         <v>53.9</v>
       </c>
       <c r="E20">
-        <v>99.2</v>
+        <v>99.3</v>
       </c>
       <c r="F20">
         <v>174.9</v>
@@ -1125,7 +1125,7 @@
         <v>66.5</v>
       </c>
       <c r="K20">
-        <v>71.5</v>
+        <v>71.400000000000006</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -1139,7 +1139,7 @@
         <v>36.200000000000003</v>
       </c>
       <c r="D21">
-        <v>58.9</v>
+        <v>589</v>
       </c>
       <c r="E21">
         <v>102.1</v>
@@ -1177,13 +1177,13 @@
         <v>55.3</v>
       </c>
       <c r="E22">
-        <v>94.6</v>
+        <v>94.5</v>
       </c>
       <c r="F22">
         <v>145.5</v>
       </c>
       <c r="G22">
-        <v>122.1</v>
+        <v>122</v>
       </c>
       <c r="H22">
         <v>119.6</v>
@@ -1195,7 +1195,7 @@
         <v>68.3</v>
       </c>
       <c r="K22">
-        <v>76.900000000000006</v>
+        <v>76.8</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -1212,13 +1212,13 @@
         <v>52.9</v>
       </c>
       <c r="E23">
-        <v>89.9</v>
+        <v>90</v>
       </c>
       <c r="F23">
         <v>130.9</v>
       </c>
       <c r="G23">
-        <v>109.5</v>
+        <v>109.4</v>
       </c>
       <c r="H23">
         <v>109.2</v>
@@ -1250,13 +1250,13 @@
         <v>82.2</v>
       </c>
       <c r="F24">
-        <v>116.4</v>
+        <v>116.5</v>
       </c>
       <c r="G24">
         <v>94.8</v>
       </c>
       <c r="H24">
-        <v>94.5</v>
+        <v>94.6</v>
       </c>
       <c r="I24">
         <v>78.7</v>
@@ -1265,7 +1265,7 @@
         <v>56.8</v>
       </c>
       <c r="K24">
-        <v>67.7</v>
+        <v>67.599999999999994</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -1282,7 +1282,7 @@
         <v>45.8</v>
       </c>
       <c r="E25">
-        <v>79</v>
+        <v>79.099999999999994</v>
       </c>
       <c r="F25">
         <v>116.2</v>
@@ -1314,10 +1314,10 @@
         <v>30.5</v>
       </c>
       <c r="D26">
-        <v>46.2</v>
+        <v>46.3</v>
       </c>
       <c r="E26">
-        <v>79.599999999999994</v>
+        <v>79.5</v>
       </c>
       <c r="F26">
         <v>138.5</v>
@@ -1343,7 +1343,7 @@
         <v>44072</v>
       </c>
       <c r="B27">
-        <v>23.1</v>
+        <v>23</v>
       </c>
       <c r="C27">
         <v>26.8</v>
@@ -1352,10 +1352,10 @@
         <v>41.3</v>
       </c>
       <c r="E27">
-        <v>69.3</v>
+        <v>69.400000000000006</v>
       </c>
       <c r="F27">
-        <v>145.80000000000001</v>
+        <v>145.9</v>
       </c>
       <c r="G27">
         <v>80.099999999999994</v>
@@ -1384,28 +1384,28 @@
         <v>22.5</v>
       </c>
       <c r="D28">
-        <v>38.9</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="E28">
-        <v>67.8</v>
+        <v>67.7</v>
       </c>
       <c r="F28">
         <v>144.69999999999999</v>
       </c>
       <c r="G28">
-        <v>67.400000000000006</v>
+        <v>67.2</v>
       </c>
       <c r="H28">
-        <v>68.3</v>
+        <v>68.2</v>
       </c>
       <c r="I28">
-        <v>58.9</v>
+        <v>58.8</v>
       </c>
       <c r="J28">
-        <v>44.9</v>
+        <v>44.8</v>
       </c>
       <c r="K28">
-        <v>55.7</v>
+        <v>55.4</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -1437,7 +1437,7 @@
         <v>60.6</v>
       </c>
       <c r="J29">
-        <v>46.2</v>
+        <v>46.3</v>
       </c>
       <c r="K29">
         <v>54.6</v>
@@ -1454,16 +1454,16 @@
         <v>30.3</v>
       </c>
       <c r="D30">
-        <v>52.2</v>
+        <v>52.3</v>
       </c>
       <c r="E30">
         <v>85.5</v>
       </c>
       <c r="F30">
-        <v>139.80000000000001</v>
+        <v>139.69999999999999</v>
       </c>
       <c r="G30">
-        <v>88.2</v>
+        <v>88.3</v>
       </c>
       <c r="H30">
         <v>87.9</v>
@@ -1472,7 +1472,7 @@
         <v>76.2</v>
       </c>
       <c r="J30">
-        <v>58.3</v>
+        <v>58.2</v>
       </c>
       <c r="K30">
         <v>68.900000000000006</v>
@@ -1501,7 +1501,7 @@
         <v>99</v>
       </c>
       <c r="H31">
-        <v>98.9</v>
+        <v>99</v>
       </c>
       <c r="I31">
         <v>86.5</v>
@@ -1510,7 +1510,7 @@
         <v>67.599999999999994</v>
       </c>
       <c r="K31">
-        <v>76.8</v>
+        <v>76.7</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -1530,13 +1530,13 @@
         <v>90.1</v>
       </c>
       <c r="F32">
-        <v>134.6</v>
+        <v>134.69999999999999</v>
       </c>
       <c r="G32">
-        <v>105.4</v>
+        <v>105.5</v>
       </c>
       <c r="H32">
-        <v>104.7</v>
+        <v>104.8</v>
       </c>
       <c r="I32">
         <v>93.5</v>
@@ -1545,7 +1545,7 @@
         <v>76.900000000000006</v>
       </c>
       <c r="K32">
-        <v>85.9</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -1559,28 +1559,28 @@
         <v>40.9</v>
       </c>
       <c r="D33">
-        <v>69.7</v>
+        <v>69.8</v>
       </c>
       <c r="E33">
-        <v>103.2</v>
+        <v>103.3</v>
       </c>
       <c r="F33">
-        <v>142.19999999999999</v>
+        <v>142.30000000000001</v>
       </c>
       <c r="G33">
-        <v>115.1</v>
+        <v>115.2</v>
       </c>
       <c r="H33">
         <v>116.5</v>
       </c>
       <c r="I33">
-        <v>104.9</v>
+        <v>105</v>
       </c>
       <c r="J33">
         <v>84.9</v>
       </c>
       <c r="K33">
-        <v>94.3</v>
+        <v>94.4</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -1594,22 +1594,22 @@
         <v>48</v>
       </c>
       <c r="D34">
-        <v>82</v>
+        <v>82.1</v>
       </c>
       <c r="E34">
         <v>118.7</v>
       </c>
       <c r="F34">
-        <v>166.3</v>
+        <v>166.4</v>
       </c>
       <c r="G34">
-        <v>142.5</v>
+        <v>142.6</v>
       </c>
       <c r="H34">
-        <v>143.19999999999999</v>
+        <v>143.4</v>
       </c>
       <c r="I34">
-        <v>128.80000000000001</v>
+        <v>128.9</v>
       </c>
       <c r="J34">
         <v>100.7</v>
@@ -1626,31 +1626,31 @@
         <v>43.4</v>
       </c>
       <c r="C35">
-        <v>59.6</v>
+        <v>59.7</v>
       </c>
       <c r="D35">
-        <v>99.6</v>
+        <v>99.7</v>
       </c>
       <c r="E35">
-        <v>140.6</v>
+        <v>140.69999999999999</v>
       </c>
       <c r="F35">
-        <v>195.2</v>
+        <v>195.4</v>
       </c>
       <c r="G35">
-        <v>172.1</v>
+        <v>172.3</v>
       </c>
       <c r="H35">
-        <v>173.4</v>
+        <v>173.5</v>
       </c>
       <c r="I35">
-        <v>153.69999999999999</v>
+        <v>153.80000000000001</v>
       </c>
       <c r="J35">
-        <v>120.2</v>
+        <v>120.3</v>
       </c>
       <c r="K35">
-        <v>133.30000000000001</v>
+        <v>133.5</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -1658,34 +1658,34 @@
         <v>44135</v>
       </c>
       <c r="B36">
-        <v>52.8</v>
+        <v>52.9</v>
       </c>
       <c r="C36">
-        <v>72.599999999999994</v>
+        <v>72.7</v>
       </c>
       <c r="D36">
-        <v>124</v>
+        <v>124.1</v>
       </c>
       <c r="E36">
-        <v>175.4</v>
+        <v>175.5</v>
       </c>
       <c r="F36">
-        <v>239.5</v>
+        <v>239.7</v>
       </c>
       <c r="G36">
-        <v>214.1</v>
+        <v>214.3</v>
       </c>
       <c r="H36">
-        <v>215.4</v>
+        <v>215.5</v>
       </c>
       <c r="I36">
-        <v>189.3</v>
+        <v>189.5</v>
       </c>
       <c r="J36">
-        <v>143.80000000000001</v>
+        <v>143.9</v>
       </c>
       <c r="K36">
-        <v>156.5</v>
+        <v>156.69999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -1696,31 +1696,31 @@
         <v>70.599999999999994</v>
       </c>
       <c r="C37">
-        <v>102</v>
+        <v>102.1</v>
       </c>
       <c r="D37">
-        <v>177.8</v>
+        <v>177.9</v>
       </c>
       <c r="E37">
-        <v>267.10000000000002</v>
+        <v>267.5</v>
       </c>
       <c r="F37">
-        <v>340</v>
+        <v>340.3</v>
       </c>
       <c r="G37">
-        <v>290.8</v>
+        <v>291</v>
       </c>
       <c r="H37">
-        <v>288</v>
+        <v>288.3</v>
       </c>
       <c r="I37">
-        <v>247.5</v>
+        <v>247.8</v>
       </c>
       <c r="J37">
-        <v>187.8</v>
+        <v>188</v>
       </c>
       <c r="K37">
-        <v>202.6</v>
+        <v>202.7</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -1731,31 +1731,31 @@
         <v>85.7</v>
       </c>
       <c r="C38">
-        <v>122.9</v>
+        <v>123</v>
       </c>
       <c r="D38">
-        <v>212.6</v>
+        <v>212.7</v>
       </c>
       <c r="E38">
-        <v>308.39999999999998</v>
+        <v>308.60000000000002</v>
       </c>
       <c r="F38">
-        <v>386.4</v>
+        <v>386.7</v>
       </c>
       <c r="G38">
-        <v>340.2</v>
+        <v>340.4</v>
       </c>
       <c r="H38">
-        <v>342.7</v>
+        <v>343</v>
       </c>
       <c r="I38">
-        <v>300.7</v>
+        <v>300.89999999999998</v>
       </c>
       <c r="J38">
-        <v>233</v>
+        <v>233.1</v>
       </c>
       <c r="K38">
-        <v>248.9</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -1763,34 +1763,34 @@
         <v>44156</v>
       </c>
       <c r="B39">
-        <v>97.3</v>
+        <v>97.5</v>
       </c>
       <c r="C39">
-        <v>137</v>
+        <v>137.1</v>
       </c>
       <c r="D39">
-        <v>226.1</v>
+        <v>226.3</v>
       </c>
       <c r="E39">
-        <v>317.89999999999998</v>
+        <v>318.3</v>
       </c>
       <c r="F39">
-        <v>425.3</v>
+        <v>425.5</v>
       </c>
       <c r="G39">
-        <v>383.8</v>
+        <v>384.1</v>
       </c>
       <c r="H39">
-        <v>382</v>
+        <v>382.4</v>
       </c>
       <c r="I39">
-        <v>338.4</v>
+        <v>338.6</v>
       </c>
       <c r="J39">
-        <v>262</v>
+        <v>262.2</v>
       </c>
       <c r="K39">
-        <v>288.3</v>
+        <v>288.39999999999998</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -1798,34 +1798,34 @@
         <v>44163</v>
       </c>
       <c r="B40">
-        <v>89.8</v>
+        <v>90</v>
       </c>
       <c r="C40">
-        <v>122.3</v>
+        <v>122.5</v>
       </c>
       <c r="D40">
-        <v>197.5</v>
+        <v>197.7</v>
       </c>
       <c r="E40">
-        <v>284.39999999999998</v>
+        <v>284.60000000000002</v>
       </c>
       <c r="F40">
-        <v>378.1</v>
+        <v>378.4</v>
       </c>
       <c r="G40">
-        <v>356.5</v>
+        <v>357</v>
       </c>
       <c r="H40">
-        <v>358.1</v>
+        <v>358.4</v>
       </c>
       <c r="I40">
-        <v>319.39999999999998</v>
+        <v>319.7</v>
       </c>
       <c r="J40">
-        <v>247.5</v>
+        <v>247.8</v>
       </c>
       <c r="K40">
-        <v>286.8</v>
+        <v>287</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -1833,34 +1833,34 @@
         <v>44170</v>
       </c>
       <c r="B41">
-        <v>122.2</v>
+        <v>122.3</v>
       </c>
       <c r="C41">
-        <v>170.2</v>
+        <v>170.4</v>
       </c>
       <c r="D41">
-        <v>263.89999999999998</v>
+        <v>264.3</v>
       </c>
       <c r="E41">
-        <v>374.8</v>
+        <v>375.5</v>
       </c>
       <c r="F41">
-        <v>485</v>
+        <v>485.7</v>
       </c>
       <c r="G41">
-        <v>450.6</v>
+        <v>451.3</v>
       </c>
       <c r="H41">
-        <v>443.3</v>
+        <v>444.2</v>
       </c>
       <c r="I41">
-        <v>385.5</v>
+        <v>386.1</v>
       </c>
       <c r="J41">
-        <v>289.39999999999998</v>
+        <v>289.89999999999998</v>
       </c>
       <c r="K41">
-        <v>331.6</v>
+        <v>332.2</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -1868,34 +1868,34 @@
         <v>44177</v>
       </c>
       <c r="B42">
-        <v>127.3</v>
+        <v>127.5</v>
       </c>
       <c r="C42">
-        <v>171.9</v>
+        <v>172</v>
       </c>
       <c r="D42">
-        <v>267</v>
+        <v>267.5</v>
       </c>
       <c r="E42">
-        <v>364.2</v>
+        <v>365</v>
       </c>
       <c r="F42">
-        <v>468.7</v>
+        <v>469.5</v>
       </c>
       <c r="G42">
-        <v>446.9</v>
+        <v>447.6</v>
       </c>
       <c r="H42">
-        <v>444</v>
+        <v>444.7</v>
       </c>
       <c r="I42">
-        <v>390.6</v>
+        <v>391.2</v>
       </c>
       <c r="J42">
-        <v>295.7</v>
+        <v>296.10000000000002</v>
       </c>
       <c r="K42">
-        <v>337.3</v>
+        <v>338</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -1909,28 +1909,28 @@
         <v>163.30000000000001</v>
       </c>
       <c r="D43">
-        <v>255.7</v>
+        <v>255.5</v>
       </c>
       <c r="E43">
-        <v>341.9</v>
+        <v>341.5</v>
       </c>
       <c r="F43">
-        <v>439.1</v>
+        <v>438.8</v>
       </c>
       <c r="G43">
-        <v>427.8</v>
+        <v>427.4</v>
       </c>
       <c r="H43">
-        <v>429.9</v>
+        <v>429.5</v>
       </c>
       <c r="I43">
-        <v>380</v>
+        <v>379.8</v>
       </c>
       <c r="J43">
-        <v>286.60000000000002</v>
+        <v>286.5</v>
       </c>
       <c r="K43">
-        <v>324.5</v>
+        <v>323.89999999999998</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -1944,28 +1944,28 @@
         <v>140.5</v>
       </c>
       <c r="D44">
-        <v>222.7</v>
+        <v>222.4</v>
       </c>
       <c r="E44">
-        <v>312.89999999999998</v>
+        <v>312.8</v>
       </c>
       <c r="F44">
-        <v>415.6</v>
+        <v>415.3</v>
       </c>
       <c r="G44">
-        <v>408.6</v>
+        <v>408.3</v>
       </c>
       <c r="H44">
-        <v>413.2</v>
+        <v>413.1</v>
       </c>
       <c r="I44">
         <v>375.2</v>
       </c>
       <c r="J44">
-        <v>294.60000000000002</v>
+        <v>294.39999999999998</v>
       </c>
       <c r="K44">
-        <v>325.89999999999998</v>
+        <v>325.8</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
@@ -1973,34 +1973,34 @@
         <v>44198</v>
       </c>
       <c r="B45">
-        <v>130.4</v>
+        <v>130.6</v>
       </c>
       <c r="C45">
-        <v>174.7</v>
+        <v>174.9</v>
       </c>
       <c r="D45">
-        <v>268.7</v>
+        <v>269</v>
       </c>
       <c r="E45">
-        <v>371.7</v>
+        <v>371.8</v>
       </c>
       <c r="F45">
-        <v>507.4</v>
+        <v>507.8</v>
       </c>
       <c r="G45">
-        <v>483.4</v>
+        <v>483.8</v>
       </c>
       <c r="H45">
-        <v>474.5</v>
+        <v>474.8</v>
       </c>
       <c r="I45">
-        <v>420.4</v>
+        <v>420.7</v>
       </c>
       <c r="J45">
-        <v>327.3</v>
+        <v>327.8</v>
       </c>
       <c r="K45">
-        <v>354.9</v>
+        <v>355.3</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -2011,19 +2011,19 @@
         <v>148.19999999999999</v>
       </c>
       <c r="C46">
-        <v>210.9</v>
+        <v>211</v>
       </c>
       <c r="D46">
-        <v>321.10000000000002</v>
+        <v>321.2</v>
       </c>
       <c r="E46">
-        <v>445.6</v>
+        <v>445.9</v>
       </c>
       <c r="F46">
         <v>578.1</v>
       </c>
       <c r="G46">
-        <v>514.79999999999995</v>
+        <v>514.70000000000005</v>
       </c>
       <c r="H46">
         <v>505.9</v>
@@ -2032,7 +2032,7 @@
         <v>445</v>
       </c>
       <c r="J46">
-        <v>337.2</v>
+        <v>337.3</v>
       </c>
       <c r="K46">
         <v>365</v>
@@ -2046,31 +2046,31 @@
         <v>130.1</v>
       </c>
       <c r="C47">
-        <v>174.8</v>
+        <v>174.7</v>
       </c>
       <c r="D47">
-        <v>256.7</v>
+        <v>256.5</v>
       </c>
       <c r="E47">
-        <v>343</v>
+        <v>342.7</v>
       </c>
       <c r="F47">
-        <v>429.6</v>
+        <v>429.1</v>
       </c>
       <c r="G47">
-        <v>386.2</v>
+        <v>385.8</v>
       </c>
       <c r="H47">
-        <v>387.4</v>
+        <v>386.9</v>
       </c>
       <c r="I47">
-        <v>351</v>
+        <v>350.7</v>
       </c>
       <c r="J47">
-        <v>271.10000000000002</v>
+        <v>270.8</v>
       </c>
       <c r="K47">
-        <v>293.89999999999998</v>
+        <v>293.60000000000002</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
@@ -2084,28 +2084,28 @@
         <v>147</v>
       </c>
       <c r="D48">
-        <v>216.7</v>
+        <v>216.8</v>
       </c>
       <c r="E48">
-        <v>280.89999999999998</v>
+        <v>281</v>
       </c>
       <c r="F48">
-        <v>331.9</v>
+        <v>331.8</v>
       </c>
       <c r="G48">
-        <v>307.5</v>
+        <v>307.39999999999998</v>
       </c>
       <c r="H48">
         <v>308.5</v>
       </c>
       <c r="I48">
-        <v>279.3</v>
+        <v>279.2</v>
       </c>
       <c r="J48">
-        <v>215</v>
+        <v>214.9</v>
       </c>
       <c r="K48">
-        <v>232.6</v>
+        <v>232.3</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
@@ -2122,25 +2122,25 @@
         <v>197.8</v>
       </c>
       <c r="E49">
-        <v>254.5</v>
+        <v>254.4</v>
       </c>
       <c r="F49">
-        <v>307.39999999999998</v>
+        <v>307.3</v>
       </c>
       <c r="G49">
-        <v>281</v>
+        <v>280.89999999999998</v>
       </c>
       <c r="H49">
-        <v>277.89999999999998</v>
+        <v>277.8</v>
       </c>
       <c r="I49">
-        <v>250.9</v>
+        <v>250.8</v>
       </c>
       <c r="J49">
-        <v>191.5</v>
+        <v>191.4</v>
       </c>
       <c r="K49">
-        <v>202</v>
+        <v>201.7</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
@@ -2148,34 +2148,34 @@
         <v>44233</v>
       </c>
       <c r="B50">
-        <v>72.599999999999994</v>
+        <v>72.5</v>
       </c>
       <c r="C50">
-        <v>101.6</v>
+        <v>101.5</v>
       </c>
       <c r="D50">
-        <v>152.1</v>
+        <v>151.9</v>
       </c>
       <c r="E50">
-        <v>190.9</v>
+        <v>190.5</v>
       </c>
       <c r="F50">
-        <v>216.1</v>
+        <v>215.9</v>
       </c>
       <c r="G50">
-        <v>196.3</v>
+        <v>196.1</v>
       </c>
       <c r="H50">
-        <v>195.3</v>
+        <v>195.1</v>
       </c>
       <c r="I50">
-        <v>176</v>
+        <v>175.8</v>
       </c>
       <c r="J50">
-        <v>136.1</v>
+        <v>135.9</v>
       </c>
       <c r="K50">
-        <v>140.30000000000001</v>
+        <v>140.1</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
@@ -2183,34 +2183,34 @@
         <v>44240</v>
       </c>
       <c r="B51">
-        <v>62.1</v>
+        <v>62</v>
       </c>
       <c r="C51">
         <v>87.1</v>
       </c>
       <c r="D51">
-        <v>127.5</v>
+        <v>127.6</v>
       </c>
       <c r="E51">
-        <v>157.30000000000001</v>
+        <v>157.4</v>
       </c>
       <c r="F51">
-        <v>187.9</v>
+        <v>187.8</v>
       </c>
       <c r="G51">
-        <v>167.9</v>
+        <v>168</v>
       </c>
       <c r="H51">
         <v>166.4</v>
       </c>
       <c r="I51">
-        <v>149.5</v>
+        <v>149.4</v>
       </c>
       <c r="J51">
         <v>112.3</v>
       </c>
       <c r="K51">
-        <v>112.9</v>
+        <v>112.7</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
@@ -2227,25 +2227,25 @@
         <v>100.5</v>
       </c>
       <c r="E52">
-        <v>133.4</v>
+        <v>133.30000000000001</v>
       </c>
       <c r="F52">
-        <v>157.69999999999999</v>
+        <v>157.6</v>
       </c>
       <c r="G52">
-        <v>136.5</v>
+        <v>136.4</v>
       </c>
       <c r="H52">
-        <v>134.5</v>
+        <v>134.4</v>
       </c>
       <c r="I52">
-        <v>120.9</v>
+        <v>120.8</v>
       </c>
       <c r="J52">
-        <v>87.6</v>
+        <v>87.5</v>
       </c>
       <c r="K52">
-        <v>84.9</v>
+        <v>84.8</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
@@ -2259,28 +2259,28 @@
         <v>68.5</v>
       </c>
       <c r="D53">
-        <v>101.3</v>
+        <v>101.2</v>
       </c>
       <c r="E53">
-        <v>130.19999999999999</v>
+        <v>130</v>
       </c>
       <c r="F53">
-        <v>157.19999999999999</v>
+        <v>157</v>
       </c>
       <c r="G53">
-        <v>134.4</v>
+        <v>134.30000000000001</v>
       </c>
       <c r="H53">
-        <v>128.30000000000001</v>
+        <v>128.1</v>
       </c>
       <c r="I53">
-        <v>116.1</v>
+        <v>116</v>
       </c>
       <c r="J53">
-        <v>83.2</v>
+        <v>83.1</v>
       </c>
       <c r="K53">
-        <v>76.099999999999994</v>
+        <v>75.900000000000006</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -2294,7 +2294,7 @@
         <v>62.4</v>
       </c>
       <c r="D54">
-        <v>93.7</v>
+        <v>93.6</v>
       </c>
       <c r="E54">
         <v>123.3</v>
@@ -2303,19 +2303,19 @@
         <v>140.69999999999999</v>
       </c>
       <c r="G54">
-        <v>132.6</v>
+        <v>132.5</v>
       </c>
       <c r="H54">
-        <v>131.6</v>
+        <v>131.5</v>
       </c>
       <c r="I54">
-        <v>116.4</v>
+        <v>116.3</v>
       </c>
       <c r="J54">
-        <v>75.400000000000006</v>
+        <v>75.3</v>
       </c>
       <c r="K54">
-        <v>67</v>
+        <v>66.900000000000006</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -2332,25 +2332,25 @@
         <v>98.4</v>
       </c>
       <c r="E55">
-        <v>130.80000000000001</v>
+        <v>130.69999999999999</v>
       </c>
       <c r="F55">
-        <v>144.4</v>
+        <v>144.30000000000001</v>
       </c>
       <c r="G55">
-        <v>128.30000000000001</v>
+        <v>128</v>
       </c>
       <c r="H55">
-        <v>126</v>
+        <v>125.8</v>
       </c>
       <c r="I55">
-        <v>111.5</v>
+        <v>111.3</v>
       </c>
       <c r="J55">
-        <v>72.599999999999994</v>
+        <v>72.5</v>
       </c>
       <c r="K55">
-        <v>65.3</v>
+        <v>65.2</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -2370,22 +2370,22 @@
         <v>155.6</v>
       </c>
       <c r="F56">
-        <v>185.8</v>
+        <v>185.7</v>
       </c>
       <c r="G56">
-        <v>165.8</v>
+        <v>1658</v>
       </c>
       <c r="H56">
-        <v>161.69999999999999</v>
+        <v>161.6</v>
       </c>
       <c r="I56">
-        <v>145.1</v>
+        <v>145</v>
       </c>
       <c r="J56">
-        <v>95</v>
+        <v>94.9</v>
       </c>
       <c r="K56">
-        <v>91.7</v>
+        <v>91.6</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
@@ -2396,28 +2396,28 @@
         <v>56.5</v>
       </c>
       <c r="C57">
-        <v>81.099999999999994</v>
+        <v>81.2</v>
       </c>
       <c r="D57">
         <v>121.5</v>
       </c>
       <c r="E57">
-        <v>161.30000000000001</v>
+        <v>161.4</v>
       </c>
       <c r="F57">
-        <v>182.2</v>
+        <v>182.3</v>
       </c>
       <c r="G57">
         <v>156.9</v>
       </c>
       <c r="H57">
-        <v>147.69999999999999</v>
+        <v>147.80000000000001</v>
       </c>
       <c r="I57">
         <v>128.30000000000001</v>
       </c>
       <c r="J57">
-        <v>70.2</v>
+        <v>70.3</v>
       </c>
       <c r="K57">
         <v>62</v>
@@ -2431,28 +2431,28 @@
         <v>54.8</v>
       </c>
       <c r="C58">
-        <v>74.3</v>
+        <v>74.2</v>
       </c>
       <c r="D58">
         <v>111.8</v>
       </c>
       <c r="E58">
-        <v>149.9</v>
+        <v>149.80000000000001</v>
       </c>
       <c r="F58">
-        <v>172.7</v>
+        <v>172.6</v>
       </c>
       <c r="G58">
         <v>145.9</v>
       </c>
       <c r="H58">
-        <v>135.9</v>
+        <v>135.80000000000001</v>
       </c>
       <c r="I58">
-        <v>112.8</v>
+        <v>112.7</v>
       </c>
       <c r="J58">
-        <v>58</v>
+        <v>57.9</v>
       </c>
       <c r="K58">
         <v>47.3</v>
@@ -2466,7 +2466,7 @@
         <v>58.3</v>
       </c>
       <c r="C59">
-        <v>80.599999999999994</v>
+        <v>80.7</v>
       </c>
       <c r="D59">
         <v>124</v>
@@ -2487,7 +2487,7 @@
         <v>110.1</v>
       </c>
       <c r="J59">
-        <v>57.9</v>
+        <v>57.8</v>
       </c>
       <c r="K59">
         <v>50</v>
@@ -2498,7 +2498,7 @@
         <v>44303</v>
       </c>
       <c r="B60">
-        <v>59.5</v>
+        <v>59.6</v>
       </c>
       <c r="C60">
         <v>84.1</v>
@@ -2507,25 +2507,25 @@
         <v>126.1</v>
       </c>
       <c r="E60">
-        <v>160.6</v>
+        <v>160.69999999999999</v>
       </c>
       <c r="F60">
         <v>164</v>
       </c>
       <c r="G60">
-        <v>142.5</v>
+        <v>142.6</v>
       </c>
       <c r="H60">
-        <v>127.7</v>
+        <v>127.8</v>
       </c>
       <c r="I60">
-        <v>101.1</v>
+        <v>101.2</v>
       </c>
       <c r="J60">
         <v>53.8</v>
       </c>
       <c r="K60">
-        <v>47.5</v>
+        <v>47.4</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -2533,13 +2533,13 @@
         <v>44310</v>
       </c>
       <c r="B61">
-        <v>55.8</v>
+        <v>55.7</v>
       </c>
       <c r="C61">
         <v>78.8</v>
       </c>
       <c r="D61">
-        <v>122.3</v>
+        <v>122.4</v>
       </c>
       <c r="E61">
         <v>147.19999999999999</v>
@@ -2551,13 +2551,13 @@
         <v>129.5</v>
       </c>
       <c r="H61">
-        <v>116.3</v>
+        <v>116.2</v>
       </c>
       <c r="I61">
         <v>90.2</v>
       </c>
       <c r="J61">
-        <v>51</v>
+        <v>50.9</v>
       </c>
       <c r="K61">
         <v>45.9</v>
@@ -2574,19 +2574,19 @@
         <v>72.099999999999994</v>
       </c>
       <c r="D62">
-        <v>113</v>
+        <v>112.9</v>
       </c>
       <c r="E62">
         <v>130.9</v>
       </c>
       <c r="F62">
-        <v>121</v>
+        <v>120.9</v>
       </c>
       <c r="G62">
-        <v>109.6</v>
+        <v>109.5</v>
       </c>
       <c r="H62">
-        <v>98.1</v>
+        <v>98</v>
       </c>
       <c r="I62">
         <v>74.099999999999994</v>
@@ -2595,7 +2595,7 @@
         <v>43</v>
       </c>
       <c r="K62">
-        <v>37.9</v>
+        <v>37.799999999999997</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
@@ -2603,7 +2603,7 @@
         <v>44324</v>
       </c>
       <c r="B63">
-        <v>46.3</v>
+        <v>46.4</v>
       </c>
       <c r="C63">
         <v>67</v>
@@ -2615,7 +2615,7 @@
         <v>115.9</v>
       </c>
       <c r="F63">
-        <v>111.2</v>
+        <v>111.1</v>
       </c>
       <c r="G63">
         <v>100.6</v>
@@ -2630,7 +2630,7 @@
         <v>42</v>
       </c>
       <c r="K63">
-        <v>37.1</v>
+        <v>37</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
@@ -2644,19 +2644,19 @@
         <v>57.9</v>
       </c>
       <c r="D64">
-        <v>88.8</v>
+        <v>88.7</v>
       </c>
       <c r="E64">
-        <v>99.7</v>
+        <v>99.6</v>
       </c>
       <c r="F64">
-        <v>104</v>
+        <v>103.9</v>
       </c>
       <c r="G64">
-        <v>91.1</v>
+        <v>91</v>
       </c>
       <c r="H64">
-        <v>82.6</v>
+        <v>82.5</v>
       </c>
       <c r="I64">
         <v>67.3</v>
@@ -2694,7 +2694,7 @@
         <v>53.6</v>
       </c>
       <c r="I65">
-        <v>42</v>
+        <v>41.9</v>
       </c>
       <c r="J65">
         <v>26.5</v>
@@ -2708,13 +2708,13 @@
         <v>44345</v>
       </c>
       <c r="B66">
-        <v>18.7</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="C66">
         <v>23.7</v>
       </c>
       <c r="D66">
-        <v>35.5</v>
+        <v>35.4</v>
       </c>
       <c r="E66">
         <v>40.4</v>
@@ -2723,7 +2723,7 @@
         <v>43.4</v>
       </c>
       <c r="G66">
-        <v>41.8</v>
+        <v>41.7</v>
       </c>
       <c r="H66">
         <v>37</v>
@@ -2749,10 +2749,10 @@
         <v>17</v>
       </c>
       <c r="D67">
-        <v>24.8</v>
+        <v>24.7</v>
       </c>
       <c r="E67">
-        <v>30.4</v>
+        <v>30.3</v>
       </c>
       <c r="F67">
         <v>33.299999999999997</v>
@@ -2784,7 +2784,7 @@
         <v>17.899999999999999</v>
       </c>
       <c r="D68">
-        <v>25.3</v>
+        <v>25.2</v>
       </c>
       <c r="E68">
         <v>31.7</v>
@@ -2793,13 +2793,13 @@
         <v>38.200000000000003</v>
       </c>
       <c r="G68">
-        <v>37.299999999999997</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="H68">
         <v>32.6</v>
       </c>
       <c r="I68">
-        <v>26.1</v>
+        <v>26</v>
       </c>
       <c r="J68">
         <v>17.2</v>
@@ -2825,7 +2825,7 @@
         <v>28</v>
       </c>
       <c r="F69">
-        <v>37.799999999999997</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="G69">
         <v>34.4</v>
@@ -2834,13 +2834,13 @@
         <v>30.6</v>
       </c>
       <c r="I69">
-        <v>25.1</v>
+        <v>25</v>
       </c>
       <c r="J69">
         <v>17.899999999999999</v>
       </c>
       <c r="K69">
-        <v>18.399999999999999</v>
+        <v>18.3</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
@@ -2851,7 +2851,7 @@
         <v>13.9</v>
       </c>
       <c r="C70">
-        <v>17.100000000000001</v>
+        <v>17</v>
       </c>
       <c r="D70">
         <v>23.1</v>
@@ -2875,7 +2875,7 @@
         <v>17.3</v>
       </c>
       <c r="K70">
-        <v>15.5</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
@@ -2895,10 +2895,10 @@
         <v>38.299999999999997</v>
       </c>
       <c r="F71">
-        <v>47.9</v>
+        <v>48</v>
       </c>
       <c r="G71">
-        <v>45.7</v>
+        <v>45.8</v>
       </c>
       <c r="H71">
         <v>39.5</v>
@@ -2921,22 +2921,22 @@
         <v>23.1</v>
       </c>
       <c r="C72">
-        <v>31.4</v>
+        <v>31.5</v>
       </c>
       <c r="D72">
-        <v>40.200000000000003</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="E72">
-        <v>52.2</v>
+        <v>52.3</v>
       </c>
       <c r="F72">
-        <v>69</v>
+        <v>69.099999999999994</v>
       </c>
       <c r="G72">
-        <v>65.099999999999994</v>
+        <v>65.2</v>
       </c>
       <c r="H72">
-        <v>54.7</v>
+        <v>54.8</v>
       </c>
       <c r="I72">
         <v>40.5</v>
@@ -2953,34 +2953,34 @@
         <v>44394</v>
       </c>
       <c r="B73">
-        <v>32.200000000000003</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="C73">
-        <v>43.3</v>
+        <v>43.4</v>
       </c>
       <c r="D73">
-        <v>54.9</v>
+        <v>55</v>
       </c>
       <c r="E73">
-        <v>68.400000000000006</v>
+        <v>68.7</v>
       </c>
       <c r="F73">
-        <v>91.8</v>
+        <v>92</v>
       </c>
       <c r="G73">
-        <v>89.2</v>
+        <v>89.4</v>
       </c>
       <c r="H73">
-        <v>71.5</v>
+        <v>71.7</v>
       </c>
       <c r="I73">
-        <v>52.4</v>
+        <v>52.5</v>
       </c>
       <c r="J73">
-        <v>37</v>
+        <v>37.1</v>
       </c>
       <c r="K73">
-        <v>32.9</v>
+        <v>33</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
@@ -2988,34 +2988,34 @@
         <v>44401</v>
       </c>
       <c r="B74">
-        <v>50.4</v>
+        <v>50.5</v>
       </c>
       <c r="C74">
-        <v>70.8</v>
+        <v>71</v>
       </c>
       <c r="D74">
-        <v>84.4</v>
+        <v>84.6</v>
       </c>
       <c r="E74">
-        <v>107.5</v>
+        <v>107.8</v>
       </c>
       <c r="F74">
-        <v>135.5</v>
+        <v>135.9</v>
       </c>
       <c r="G74">
-        <v>131.5</v>
+        <v>131.80000000000001</v>
       </c>
       <c r="H74">
-        <v>108.2</v>
+        <v>108.5</v>
       </c>
       <c r="I74">
-        <v>77.7</v>
+        <v>77.900000000000006</v>
       </c>
       <c r="J74">
-        <v>56.1</v>
+        <v>56.2</v>
       </c>
       <c r="K74">
-        <v>47.3</v>
+        <v>47.4</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
@@ -3023,34 +3023,34 @@
         <v>44408</v>
       </c>
       <c r="B75">
-        <v>76.099999999999994</v>
+        <v>76.3</v>
       </c>
       <c r="C75">
-        <v>108.6</v>
+        <v>108.9</v>
       </c>
       <c r="D75">
-        <v>122.9</v>
+        <v>123.2</v>
       </c>
       <c r="E75">
-        <v>153.19999999999999</v>
+        <v>153.5</v>
       </c>
       <c r="F75">
-        <v>193.9</v>
+        <v>194.5</v>
       </c>
       <c r="G75">
-        <v>183.7</v>
+        <v>184.2</v>
       </c>
       <c r="H75">
-        <v>152.9</v>
+        <v>153.30000000000001</v>
       </c>
       <c r="I75">
-        <v>109.3</v>
+        <v>109.7</v>
       </c>
       <c r="J75">
-        <v>80</v>
+        <v>80.3</v>
       </c>
       <c r="K75">
-        <v>71</v>
+        <v>71.099999999999994</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
@@ -3058,34 +3058,34 @@
         <v>44415</v>
       </c>
       <c r="B76">
-        <v>102</v>
+        <v>102.4</v>
       </c>
       <c r="C76">
-        <v>145.80000000000001</v>
+        <v>146.19999999999999</v>
       </c>
       <c r="D76">
-        <v>163.9</v>
+        <v>164.2</v>
       </c>
       <c r="E76">
-        <v>200.7</v>
+        <v>201.3</v>
       </c>
       <c r="F76">
-        <v>248.7</v>
+        <v>249.3</v>
       </c>
       <c r="G76">
-        <v>242.2</v>
+        <v>243</v>
       </c>
       <c r="H76">
-        <v>208.7</v>
+        <v>209.4</v>
       </c>
       <c r="I76">
-        <v>156.19999999999999</v>
+        <v>156.6</v>
       </c>
       <c r="J76">
-        <v>116.1</v>
+        <v>116.4</v>
       </c>
       <c r="K76">
-        <v>111.3</v>
+        <v>111.5</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
@@ -3093,34 +3093,34 @@
         <v>44422</v>
       </c>
       <c r="B77">
-        <v>129.5</v>
+        <v>130</v>
       </c>
       <c r="C77">
-        <v>201.6</v>
+        <v>202.2</v>
       </c>
       <c r="D77">
-        <v>217.9</v>
+        <v>219</v>
       </c>
       <c r="E77">
-        <v>253.7</v>
+        <v>254.6</v>
       </c>
       <c r="F77">
-        <v>269.39999999999998</v>
+        <v>270.10000000000002</v>
       </c>
       <c r="G77">
-        <v>270.39999999999998</v>
+        <v>271</v>
       </c>
       <c r="H77">
-        <v>233.8</v>
+        <v>234.4</v>
       </c>
       <c r="I77">
-        <v>173.2</v>
+        <v>173.7</v>
       </c>
       <c r="J77">
-        <v>129.9</v>
+        <v>130.19999999999999</v>
       </c>
       <c r="K77">
-        <v>118.6</v>
+        <v>119</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
@@ -3128,34 +3128,34 @@
         <v>44429</v>
       </c>
       <c r="B78">
-        <v>140.80000000000001</v>
+        <v>141.4</v>
       </c>
       <c r="C78">
-        <v>248</v>
+        <v>249.2</v>
       </c>
       <c r="D78">
-        <v>275.5</v>
+        <v>277.10000000000002</v>
       </c>
       <c r="E78">
-        <v>288.5</v>
+        <v>290.10000000000002</v>
       </c>
       <c r="F78">
-        <v>257.60000000000002</v>
+        <v>258.8</v>
       </c>
       <c r="G78">
-        <v>264.2</v>
+        <v>265.39999999999998</v>
       </c>
       <c r="H78">
-        <v>227.3</v>
+        <v>228.2</v>
       </c>
       <c r="I78">
-        <v>170.4</v>
+        <v>171.4</v>
       </c>
       <c r="J78">
-        <v>132.80000000000001</v>
+        <v>133.4</v>
       </c>
       <c r="K78">
-        <v>119.5</v>
+        <v>119.9</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
@@ -3163,34 +3163,34 @@
         <v>44436</v>
       </c>
       <c r="B79">
-        <v>173.6</v>
+        <v>174.8</v>
       </c>
       <c r="C79">
-        <v>312.8</v>
+        <v>315</v>
       </c>
       <c r="D79">
-        <v>362.8</v>
+        <v>366.4</v>
       </c>
       <c r="E79">
-        <v>373.6</v>
+        <v>377.8</v>
       </c>
       <c r="F79">
-        <v>311.5</v>
+        <v>313.8</v>
       </c>
       <c r="G79">
-        <v>315.60000000000002</v>
+        <v>318.2</v>
       </c>
       <c r="H79">
-        <v>271.89999999999998</v>
+        <v>274.3</v>
       </c>
       <c r="I79">
-        <v>203.6</v>
+        <v>205.2</v>
       </c>
       <c r="J79">
-        <v>155.69999999999999</v>
+        <v>156.9</v>
       </c>
       <c r="K79">
-        <v>139.80000000000001</v>
+        <v>140.69999999999999</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
@@ -3198,34 +3198,34 @@
         <v>44443</v>
       </c>
       <c r="B80">
-        <v>149.9</v>
+        <v>150.6</v>
       </c>
       <c r="C80">
-        <v>288</v>
+        <v>289.2</v>
       </c>
       <c r="D80">
-        <v>334.4</v>
+        <v>335.8</v>
       </c>
       <c r="E80">
-        <v>343.8</v>
+        <v>345.9</v>
       </c>
       <c r="F80">
-        <v>262.10000000000002</v>
+        <v>264</v>
       </c>
       <c r="G80">
-        <v>270.7</v>
+        <v>272.39999999999998</v>
       </c>
       <c r="H80">
-        <v>235.2</v>
+        <v>236.7</v>
       </c>
       <c r="I80">
-        <v>176.4</v>
+        <v>177.6</v>
       </c>
       <c r="J80">
-        <v>138.69999999999999</v>
+        <v>139.69999999999999</v>
       </c>
       <c r="K80">
-        <v>126.7</v>
+        <v>127.6</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
@@ -3233,34 +3233,34 @@
         <v>44450</v>
       </c>
       <c r="B81">
-        <v>148</v>
+        <v>147.9</v>
       </c>
       <c r="C81">
-        <v>277</v>
+        <v>277.3</v>
       </c>
       <c r="D81">
-        <v>323.60000000000002</v>
+        <v>323.10000000000002</v>
       </c>
       <c r="E81">
-        <v>335.3</v>
+        <v>334.3</v>
       </c>
       <c r="F81">
-        <v>263.5</v>
+        <v>262.8</v>
       </c>
       <c r="G81">
-        <v>273.3</v>
+        <v>272.7</v>
       </c>
       <c r="H81">
-        <v>240.4</v>
+        <v>240.1</v>
       </c>
       <c r="I81">
-        <v>180.5</v>
+        <v>180.4</v>
       </c>
       <c r="J81">
-        <v>140.9</v>
+        <v>141</v>
       </c>
       <c r="K81">
-        <v>129.30000000000001</v>
+        <v>129.4</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
@@ -3268,34 +3268,34 @@
         <v>44457</v>
       </c>
       <c r="B82">
-        <v>165.2</v>
+        <v>166.2</v>
       </c>
       <c r="C82">
-        <v>291.8</v>
+        <v>293.10000000000002</v>
       </c>
       <c r="D82">
-        <v>318.8</v>
+        <v>319.5</v>
       </c>
       <c r="E82">
-        <v>336.5</v>
+        <v>337.2</v>
       </c>
       <c r="F82">
-        <v>289.8</v>
+        <v>290.89999999999998</v>
       </c>
       <c r="G82">
-        <v>306.2</v>
+        <v>307.10000000000002</v>
       </c>
       <c r="H82">
-        <v>272.39999999999998</v>
+        <v>273.3</v>
       </c>
       <c r="I82">
-        <v>210.8</v>
+        <v>211.5</v>
       </c>
       <c r="J82">
-        <v>165.5</v>
+        <v>166.3</v>
       </c>
       <c r="K82">
-        <v>152.5</v>
+        <v>153</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
@@ -3303,34 +3303,34 @@
         <v>44464</v>
       </c>
       <c r="B83">
-        <v>130.69999999999999</v>
+        <v>131.30000000000001</v>
       </c>
       <c r="C83">
-        <v>237</v>
+        <v>238.6</v>
       </c>
       <c r="D83">
-        <v>248.1</v>
+        <v>249.4</v>
       </c>
       <c r="E83">
-        <v>258.60000000000002</v>
+        <v>259.89999999999998</v>
       </c>
       <c r="F83">
-        <v>209.1</v>
+        <v>209.9</v>
       </c>
       <c r="G83">
-        <v>230.6</v>
+        <v>231.8</v>
       </c>
       <c r="H83">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="I83">
-        <v>161.1</v>
+        <v>162</v>
       </c>
       <c r="J83">
-        <v>132.9</v>
+        <v>133.5</v>
       </c>
       <c r="K83">
-        <v>123.7</v>
+        <v>124.5</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
@@ -3338,34 +3338,34 @@
         <v>44471</v>
       </c>
       <c r="B84">
-        <v>136.1</v>
+        <v>137.6</v>
       </c>
       <c r="C84">
-        <v>252.1</v>
+        <v>254.3</v>
       </c>
       <c r="D84">
-        <v>255.2</v>
+        <v>257.7</v>
       </c>
       <c r="E84">
-        <v>260.10000000000002</v>
+        <v>262.89999999999998</v>
       </c>
       <c r="F84">
-        <v>218.5</v>
+        <v>220.2</v>
       </c>
       <c r="G84">
-        <v>253.3</v>
+        <v>255.1</v>
       </c>
       <c r="H84">
-        <v>227.8</v>
+        <v>229.5</v>
       </c>
       <c r="I84">
-        <v>180.6</v>
+        <v>181.9</v>
       </c>
       <c r="J84">
-        <v>149.19999999999999</v>
+        <v>150.5</v>
       </c>
       <c r="K84">
-        <v>142.1</v>
+        <v>143.1</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
@@ -3373,34 +3373,34 @@
         <v>44478</v>
       </c>
       <c r="B85">
-        <v>104.4</v>
+        <v>105.1</v>
       </c>
       <c r="C85">
-        <v>196.8</v>
+        <v>197.8</v>
       </c>
       <c r="D85">
-        <v>197.3</v>
+        <v>197.9</v>
       </c>
       <c r="E85">
-        <v>203.1</v>
+        <v>204</v>
       </c>
       <c r="F85">
-        <v>165.9</v>
+        <v>166.9</v>
       </c>
       <c r="G85">
-        <v>195.9</v>
+        <v>196.9</v>
       </c>
       <c r="H85">
-        <v>177.6</v>
+        <v>178.6</v>
       </c>
       <c r="I85">
-        <v>143.30000000000001</v>
+        <v>144.30000000000001</v>
       </c>
       <c r="J85">
-        <v>122.5</v>
+        <v>123.3</v>
       </c>
       <c r="K85">
-        <v>115.1</v>
+        <v>115.6</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
@@ -3408,34 +3408,34 @@
         <v>44485</v>
       </c>
       <c r="B86">
-        <v>85.7</v>
+        <v>86.8</v>
       </c>
       <c r="C86">
-        <v>158.4</v>
+        <v>159.5</v>
       </c>
       <c r="D86">
-        <v>148.69999999999999</v>
+        <v>150.1</v>
       </c>
       <c r="E86">
-        <v>157.6</v>
+        <v>159.4</v>
       </c>
       <c r="F86">
-        <v>133.4</v>
+        <v>135.1</v>
       </c>
       <c r="G86">
-        <v>158.69999999999999</v>
+        <v>160.5</v>
       </c>
       <c r="H86">
-        <v>145</v>
+        <v>146.69999999999999</v>
       </c>
       <c r="I86">
-        <v>118</v>
+        <v>119.6</v>
       </c>
       <c r="J86">
-        <v>100.3</v>
+        <v>101.7</v>
       </c>
       <c r="K86">
-        <v>97.3</v>
+        <v>99</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
@@ -3443,34 +3443,69 @@
         <v>44492</v>
       </c>
       <c r="B87">
-        <v>79.2</v>
+        <v>83.7</v>
       </c>
       <c r="C87">
-        <v>144.4</v>
+        <v>153.4</v>
       </c>
       <c r="D87">
-        <v>125.9</v>
+        <v>134.1</v>
       </c>
       <c r="E87">
-        <v>129.69999999999999</v>
+        <v>137.9</v>
       </c>
       <c r="F87">
-        <v>120</v>
+        <v>126.2</v>
       </c>
       <c r="G87">
-        <v>144.80000000000001</v>
+        <v>152.19999999999999</v>
       </c>
       <c r="H87">
-        <v>130.80000000000001</v>
+        <v>1383</v>
       </c>
       <c r="I87">
-        <v>109.5</v>
+        <v>115.9</v>
       </c>
       <c r="J87">
-        <v>90.5</v>
+        <v>95.8</v>
       </c>
       <c r="K87">
-        <v>88.2</v>
+        <v>92.9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>44499</v>
+      </c>
+      <c r="B88">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="C88">
+        <v>146.19999999999999</v>
+      </c>
+      <c r="D88">
+        <v>118.8</v>
+      </c>
+      <c r="E88">
+        <v>121.4</v>
+      </c>
+      <c r="F88">
+        <v>118</v>
+      </c>
+      <c r="G88">
+        <v>140.30000000000001</v>
+      </c>
+      <c r="H88">
+        <v>125.8</v>
+      </c>
+      <c r="I88">
+        <v>103.9</v>
+      </c>
+      <c r="J88">
+        <v>82.8</v>
+      </c>
+      <c r="K88">
+        <v>81.900000000000006</v>
       </c>
     </row>
   </sheetData>
@@ -3482,8 +3517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4571D5CF-E411-3B4E-8AAF-5136E7E11E59}">
   <dimension ref="A1:K85"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="K52" sqref="A44:K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3619,317 +3654,317 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>44436</v>
+        <v>44443</v>
       </c>
       <c r="B44">
-        <v>173.6</v>
+        <v>150.6</v>
       </c>
       <c r="C44">
-        <v>312.8</v>
+        <v>289.2</v>
       </c>
       <c r="D44">
-        <v>362.8</v>
+        <v>335.8</v>
       </c>
       <c r="E44">
-        <v>373.6</v>
+        <v>345.9</v>
       </c>
       <c r="F44">
-        <v>311.5</v>
+        <v>264</v>
       </c>
       <c r="G44">
-        <v>315.60000000000002</v>
+        <v>272.39999999999998</v>
       </c>
       <c r="H44">
-        <v>271.89999999999998</v>
+        <v>236.7</v>
       </c>
       <c r="I44">
-        <v>203.6</v>
+        <v>177.6</v>
       </c>
       <c r="J44">
-        <v>155.69999999999999</v>
+        <v>139.69999999999999</v>
       </c>
       <c r="K44">
-        <v>139.80000000000001</v>
+        <v>127.6</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>44443</v>
+        <v>44450</v>
       </c>
       <c r="B45">
-        <v>149.9</v>
+        <v>147.9</v>
       </c>
       <c r="C45">
-        <v>288</v>
+        <v>277.3</v>
       </c>
       <c r="D45">
-        <v>334.4</v>
+        <v>323.10000000000002</v>
       </c>
       <c r="E45">
-        <v>343.8</v>
+        <v>334.3</v>
       </c>
       <c r="F45">
-        <v>262.10000000000002</v>
+        <v>262.8</v>
       </c>
       <c r="G45">
-        <v>270.7</v>
+        <v>272.7</v>
       </c>
       <c r="H45">
-        <v>235.2</v>
+        <v>240.1</v>
       </c>
       <c r="I45">
-        <v>176.4</v>
+        <v>180.4</v>
       </c>
       <c r="J45">
-        <v>138.69999999999999</v>
+        <v>141</v>
       </c>
       <c r="K45">
-        <v>126.7</v>
+        <v>129.4</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>44450</v>
+        <v>44457</v>
       </c>
       <c r="B46">
-        <v>148</v>
+        <v>166.2</v>
       </c>
       <c r="C46">
-        <v>277</v>
+        <v>293.10000000000002</v>
       </c>
       <c r="D46">
-        <v>323.60000000000002</v>
+        <v>319.5</v>
       </c>
       <c r="E46">
-        <v>335.3</v>
+        <v>337.2</v>
       </c>
       <c r="F46">
-        <v>263.5</v>
+        <v>290.89999999999998</v>
       </c>
       <c r="G46">
+        <v>307.10000000000002</v>
+      </c>
+      <c r="H46">
         <v>273.3</v>
       </c>
-      <c r="H46">
-        <v>240.4</v>
-      </c>
       <c r="I46">
-        <v>180.5</v>
+        <v>211.5</v>
       </c>
       <c r="J46">
-        <v>140.9</v>
+        <v>166.3</v>
       </c>
       <c r="K46">
-        <v>129.30000000000001</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>44457</v>
+        <v>44464</v>
       </c>
       <c r="B47">
-        <v>165.2</v>
+        <v>131.30000000000001</v>
       </c>
       <c r="C47">
-        <v>291.8</v>
+        <v>238.6</v>
       </c>
       <c r="D47">
-        <v>318.8</v>
+        <v>249.4</v>
       </c>
       <c r="E47">
-        <v>336.5</v>
+        <v>259.89999999999998</v>
       </c>
       <c r="F47">
-        <v>289.8</v>
+        <v>209.9</v>
       </c>
       <c r="G47">
-        <v>306.2</v>
+        <v>231.8</v>
       </c>
       <c r="H47">
-        <v>272.39999999999998</v>
+        <v>207</v>
       </c>
       <c r="I47">
-        <v>210.8</v>
+        <v>162</v>
       </c>
       <c r="J47">
-        <v>165.5</v>
+        <v>133.5</v>
       </c>
       <c r="K47">
-        <v>152.5</v>
+        <v>124.5</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>44464</v>
+        <v>44471</v>
       </c>
       <c r="B48">
-        <v>130.69999999999999</v>
+        <v>137.6</v>
       </c>
       <c r="C48">
-        <v>237</v>
+        <v>254.3</v>
       </c>
       <c r="D48">
-        <v>248.1</v>
+        <v>257.7</v>
       </c>
       <c r="E48">
-        <v>258.60000000000002</v>
+        <v>262.89999999999998</v>
       </c>
       <c r="F48">
-        <v>209.1</v>
+        <v>220.2</v>
       </c>
       <c r="G48">
-        <v>230.6</v>
+        <v>255.1</v>
       </c>
       <c r="H48">
-        <v>206</v>
+        <v>229.5</v>
       </c>
       <c r="I48">
-        <v>161.1</v>
+        <v>181.9</v>
       </c>
       <c r="J48">
-        <v>132.9</v>
+        <v>150.5</v>
       </c>
       <c r="K48">
-        <v>123.7</v>
+        <v>143.1</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>44471</v>
+        <v>44478</v>
       </c>
       <c r="B49">
-        <v>136.1</v>
+        <v>105.1</v>
       </c>
       <c r="C49">
-        <v>252.1</v>
+        <v>197.8</v>
       </c>
       <c r="D49">
-        <v>255.2</v>
+        <v>197.9</v>
       </c>
       <c r="E49">
-        <v>260.10000000000002</v>
+        <v>204</v>
       </c>
       <c r="F49">
-        <v>218.5</v>
+        <v>166.9</v>
       </c>
       <c r="G49">
-        <v>253.3</v>
+        <v>196.9</v>
       </c>
       <c r="H49">
-        <v>227.8</v>
+        <v>178.6</v>
       </c>
       <c r="I49">
-        <v>180.6</v>
+        <v>144.30000000000001</v>
       </c>
       <c r="J49">
-        <v>149.19999999999999</v>
+        <v>123.3</v>
       </c>
       <c r="K49">
-        <v>142.1</v>
+        <v>115.6</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>44478</v>
+        <v>44485</v>
       </c>
       <c r="B50">
-        <v>104.4</v>
+        <v>86.8</v>
       </c>
       <c r="C50">
-        <v>196.8</v>
+        <v>159.5</v>
       </c>
       <c r="D50">
-        <v>197.3</v>
+        <v>150.1</v>
       </c>
       <c r="E50">
-        <v>203.1</v>
+        <v>159.4</v>
       </c>
       <c r="F50">
-        <v>165.9</v>
+        <v>135.1</v>
       </c>
       <c r="G50">
-        <v>195.9</v>
+        <v>160.5</v>
       </c>
       <c r="H50">
-        <v>177.6</v>
+        <v>146.69999999999999</v>
       </c>
       <c r="I50">
-        <v>143.30000000000001</v>
+        <v>119.6</v>
       </c>
       <c r="J50">
-        <v>122.5</v>
+        <v>101.7</v>
       </c>
       <c r="K50">
-        <v>115.1</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>44485</v>
+        <v>44492</v>
       </c>
       <c r="B51">
-        <v>85.7</v>
+        <v>83.7</v>
       </c>
       <c r="C51">
-        <v>158.4</v>
+        <v>153.4</v>
       </c>
       <c r="D51">
-        <v>148.69999999999999</v>
+        <v>134.1</v>
       </c>
       <c r="E51">
-        <v>157.6</v>
+        <v>137.9</v>
       </c>
       <c r="F51">
-        <v>133.4</v>
+        <v>126.2</v>
       </c>
       <c r="G51">
-        <v>158.69999999999999</v>
+        <v>152.19999999999999</v>
       </c>
       <c r="H51">
-        <v>145</v>
+        <v>1383</v>
       </c>
       <c r="I51">
-        <v>118</v>
+        <v>115.9</v>
       </c>
       <c r="J51">
-        <v>100.3</v>
+        <v>95.8</v>
       </c>
       <c r="K51">
-        <v>97.3</v>
+        <v>92.9</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>44492</v>
+        <v>44499</v>
       </c>
       <c r="B52">
-        <v>79.2</v>
+        <v>74.599999999999994</v>
       </c>
       <c r="C52">
-        <v>144.4</v>
+        <v>146.19999999999999</v>
       </c>
       <c r="D52">
-        <v>125.9</v>
+        <v>118.8</v>
       </c>
       <c r="E52">
-        <v>129.69999999999999</v>
+        <v>121.4</v>
       </c>
       <c r="F52">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G52">
-        <v>144.80000000000001</v>
+        <v>140.30000000000001</v>
       </c>
       <c r="H52">
-        <v>130.80000000000001</v>
+        <v>125.8</v>
       </c>
       <c r="I52">
-        <v>109.5</v>
+        <v>103.9</v>
       </c>
       <c r="J52">
-        <v>90.5</v>
+        <v>82.8</v>
       </c>
       <c r="K52">
-        <v>88.2</v>
+        <v>81.900000000000006</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update missing decimal 12-15
</commit_message>
<xml_diff>
--- a/case_data.xlsx
+++ b/case_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timwiemken/Library/Mobile Documents/com~apple~CloudDocs/Work/Pfizer/COVID pediatric case count/count github/covid-agegroups/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pfizer-my.sharepoint.com/personal/wiemkt_pfizer_com/Documents/Documents/Research/covid-agegroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64ED935-E650-9348-B66A-D5737C8B2C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{D64ED935-E650-9348-B66A-D5737C8B2C53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{05600289-3CF8-45D6-BC45-206A6EAA2611}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="500" windowWidth="27600" windowHeight="17500" xr2:uid="{CC2C058F-5A66-1E4E-8340-2D9DC2FB7952}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{CC2C058F-5A66-1E4E-8340-2D9DC2FB7952}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -423,12 +423,12 @@
   <dimension ref="A1:K88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +463,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>43897</v>
       </c>
@@ -498,7 +498,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>43904</v>
       </c>
@@ -533,7 +533,7 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>43911</v>
       </c>
@@ -568,7 +568,7 @@
         <v>36.200000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>43918</v>
       </c>
@@ -603,7 +603,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>43925</v>
       </c>
@@ -638,7 +638,7 @@
         <v>95.1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>43932</v>
       </c>
@@ -673,7 +673,7 @@
         <v>121.3</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>43939</v>
       </c>
@@ -708,7 +708,7 @@
         <v>118.5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>43946</v>
       </c>
@@ -743,7 +743,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>43953</v>
       </c>
@@ -778,7 +778,7 @@
         <v>103.7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>43960</v>
       </c>
@@ -813,7 +813,7 @@
         <v>83.3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>43967</v>
       </c>
@@ -848,7 +848,7 @@
         <v>76.7</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>43974</v>
       </c>
@@ -883,7 +883,7 @@
         <v>65.099999999999994</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>43981</v>
       </c>
@@ -918,7 +918,7 @@
         <v>57.5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>43988</v>
       </c>
@@ -953,7 +953,7 @@
         <v>48.9</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>43995</v>
       </c>
@@ -988,7 +988,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>44002</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>51.4</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>44009</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>66.8</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>44016</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>44023</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>71.400000000000006</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>44030</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>36.200000000000003</v>
       </c>
       <c r="D21">
-        <v>589</v>
+        <v>58.9</v>
       </c>
       <c r="E21">
         <v>102.1</v>
@@ -1163,7 +1163,7 @@
         <v>78.400000000000006</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>44037</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>76.8</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>44044</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>74.8</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>44051</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>67.599999999999994</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>44058</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>66.5</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>44065</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>72.2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>44072</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>58.7</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>44079</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>55.4</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>44086</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>54.6</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>44093</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>68.900000000000006</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>44100</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>76.7</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>44107</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>44114</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>94.4</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>44121</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>113.9</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>44128</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>133.5</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>44135</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>156.69999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>44142</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>202.7</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>44149</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>44156</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>288.39999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>44163</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>44170</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>332.2</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>44177</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>44184</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>323.89999999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>44191</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>325.8</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>44198</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>355.3</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>44205</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>44212</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>293.60000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>44219</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>232.3</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>44226</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>201.7</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>44233</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>140.1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>44240</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>112.7</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>44247</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>84.8</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>44254</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>75.900000000000006</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>44261</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>66.900000000000006</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>44268</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>65.2</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>44275</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>91.6</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>44282</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>44289</v>
       </c>
@@ -2458,7 +2458,7 @@
         <v>47.3</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>44296</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>44303</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>47.4</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>44310</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>45.9</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
         <v>44317</v>
       </c>
@@ -2598,7 +2598,7 @@
         <v>37.799999999999997</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A63" s="1">
         <v>44324</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64" s="1">
         <v>44331</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>35.9</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A65" s="1">
         <v>44338</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A66" s="1">
         <v>44345</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>18.8</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A67" s="1">
         <v>44352</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>15.1</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A68" s="1">
         <v>44359</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A69" s="1">
         <v>44366</v>
       </c>
@@ -2843,7 +2843,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A70" s="1">
         <v>44373</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A71" s="1">
         <v>44380</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A72" s="1">
         <v>44387</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>24.6</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A73" s="1">
         <v>44394</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A74" s="1">
         <v>44401</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>47.4</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A75" s="1">
         <v>44408</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>71.099999999999994</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A76" s="1">
         <v>44415</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>111.5</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A77" s="1">
         <v>44422</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A78" s="1">
         <v>44429</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>119.9</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A79" s="1">
         <v>44436</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>140.69999999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A80" s="1">
         <v>44443</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>127.6</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A81" s="1">
         <v>44450</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>129.4</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A82" s="1">
         <v>44457</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A83" s="1">
         <v>44464</v>
       </c>
@@ -3333,7 +3333,7 @@
         <v>124.5</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84" s="1">
         <v>44471</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>143.1</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" s="1">
         <v>44478</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>115.6</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86" s="1">
         <v>44485</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87" s="1">
         <v>44492</v>
       </c>
@@ -3473,7 +3473,7 @@
         <v>92.9</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88" s="1">
         <v>44499</v>
       </c>
@@ -3521,138 +3521,138 @@
       <selection activeCell="K52" sqref="A44:K52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>44443</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>127.6</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>44450</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>129.4</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>44457</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>44464</v>
       </c>
@@ -3792,7 +3792,7 @@
         <v>124.5</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>44471</v>
       </c>
@@ -3827,7 +3827,7 @@
         <v>143.1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>44478</v>
       </c>
@@ -3862,7 +3862,7 @@
         <v>115.6</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>44485</v>
       </c>
@@ -3897,7 +3897,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>44492</v>
       </c>
@@ -3932,7 +3932,7 @@
         <v>92.9</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>44499</v>
       </c>
@@ -3967,103 +3967,103 @@
         <v>81.900000000000006</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64" s="1"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65" s="1"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A66" s="1"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A69" s="1"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A70" s="1"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A71" s="1"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A72" s="1"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A73" s="1"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" s="1"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A75" s="1"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A76" s="1"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A77" s="1"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A78" s="1"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A79" s="1"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A80" s="1"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A81" s="1"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A82" s="1"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A83" s="1"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A84" s="1"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A85" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated decomal for 30-39
</commit_message>
<xml_diff>
--- a/case_data.xlsx
+++ b/case_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pfizer-my.sharepoint.com/personal/wiemkt_pfizer_com/Documents/Documents/Research/covid-agegroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{D64ED935-E650-9348-B66A-D5737C8B2C53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{05600289-3CF8-45D6-BC45-206A6EAA2611}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{D64ED935-E650-9348-B66A-D5737C8B2C53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{22C23189-DBDE-4259-8457-2DE14694E3AC}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{CC2C058F-5A66-1E4E-8340-2D9DC2FB7952}"/>
   </bookViews>
@@ -422,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14FFA509-206F-304C-A5FE-F366C177BBC6}">
   <dimension ref="A1:K88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
@@ -2373,7 +2373,7 @@
         <v>185.7</v>
       </c>
       <c r="G56">
-        <v>1658</v>
+        <v>165.8</v>
       </c>
       <c r="H56">
         <v>161.6</v>

</xml_diff>